<commit_message>
Results of scalability tests
</commit_message>
<xml_diff>
--- a/input/core_algorithms_2022/Experiment_results.xlsx
+++ b/input/core_algorithms_2022/Experiment_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_Devel\Repos\repos-2020-06\model-interplay-monitoring-code\input\core_algorithms_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD316F3-1ABA-451E-BD61-F7C2B23F700F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD95F099-6B2E-4818-BA07-559557704DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
+    <workbookView xWindow="7065" yWindow="2400" windowWidth="20760" windowHeight="11505" activeTab="2" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
   </bookViews>
   <sheets>
     <sheet name="modelSize" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="86">
   <si>
     <t>States</t>
   </si>
@@ -285,6 +285,15 @@
   </si>
   <si>
     <t>NB! The non-deterministic nature of Java GC means that memory consumption with the same inputs may vary significantly (up to multiple GB in some tests).</t>
+  </si>
+  <si>
+    <t>NB! The non-deterministic nature of Java GC means that memory consumption with the same inputs may vary significantly (up to multiple GB in some tests) and is therefore currently not measured.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>14/7</t>
   </si>
 </sst>
 </file>
@@ -437,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -473,9 +482,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -505,6 +525,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D70222-B554-4BB9-8CB5-22FD4E14CBB3}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -833,7 +863,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>82</v>
       </c>
     </row>
@@ -843,36 +873,36 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="18" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
@@ -893,7 +923,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>0</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -905,9 +935,22 @@
       <c r="D6" s="14">
         <v>1</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4">
+        <v>2.7E-2</v>
+      </c>
+      <c r="F6">
+        <v>54</v>
+      </c>
       <c r="G6" s="3"/>
-      <c r="J6" s="1"/>
+      <c r="H6">
+        <v>9.4E-2</v>
+      </c>
+      <c r="I6">
+        <v>32.457999999999998</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.255</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -922,9 +965,22 @@
       <c r="D7" s="14">
         <v>2</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F7">
+        <v>272</v>
+      </c>
       <c r="G7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="H7">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="I7">
+        <v>35.712000000000003</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.28100000000000003</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -939,9 +995,22 @@
       <c r="D8" s="14">
         <v>3</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4">
+        <v>0.152</v>
+      </c>
+      <c r="F8">
+        <v>1026</v>
+      </c>
       <c r="G8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="H8">
+        <v>0.115</v>
+      </c>
+      <c r="I8">
+        <v>35.018999999999998</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.32700000000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -956,9 +1025,22 @@
       <c r="D9" s="14">
         <v>4</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="F9">
+        <v>3484</v>
+      </c>
       <c r="G9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="H9">
+        <v>0.111</v>
+      </c>
+      <c r="I9">
+        <v>46.719000000000001</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.31</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -973,9 +1055,22 @@
       <c r="D10" s="14">
         <v>5</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4">
+        <v>2.3519999999999999</v>
+      </c>
+      <c r="F10">
+        <v>11278</v>
+      </c>
       <c r="G10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="H10">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I10">
+        <v>59.615000000000002</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.307</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -990,9 +1085,22 @@
       <c r="D11" s="14">
         <v>6</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4">
+        <v>7.577</v>
+      </c>
+      <c r="F11">
+        <v>35560</v>
+      </c>
       <c r="G11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="H11">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="I11">
+        <v>15.631</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.27900000000000003</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -1007,9 +1115,22 @@
       <c r="D12" s="14">
         <v>7</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4">
+        <v>29.707999999999998</v>
+      </c>
+      <c r="F12">
+        <v>110298</v>
+      </c>
       <c r="G12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="H12">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="I12">
+        <v>12.218999999999999</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.251</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -1017,33 +1138,33 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="18" t="s">
+      <c r="C15" s="23"/>
+      <c r="D15" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="24" t="s">
+      <c r="E15" s="23"/>
+      <c r="F15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="18" t="s">
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="19"/>
-      <c r="L15" s="20"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="23"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
@@ -1056,7 +1177,7 @@
       <c r="E16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="25"/>
+      <c r="F16" s="28"/>
       <c r="G16" s="7" t="s">
         <v>12</v>
       </c>
@@ -1077,7 +1198,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <v>0</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -1095,9 +1216,22 @@
       <c r="F17" s="14">
         <v>1</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="4">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="H17">
+        <v>80</v>
+      </c>
       <c r="I17" s="3"/>
-      <c r="L17" s="1"/>
+      <c r="J17">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="K17">
+        <v>29.193000000000001</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0.28699999999999998</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -1118,9 +1252,22 @@
       <c r="F18" s="14">
         <v>2</v>
       </c>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="H18">
+        <v>462</v>
+      </c>
       <c r="I18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="J18">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="K18">
+        <v>34.284999999999997</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0.30399999999999999</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -1141,9 +1288,22 @@
       <c r="F19" s="14">
         <v>3</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4">
+        <v>0.83</v>
+      </c>
+      <c r="H19">
+        <v>1824</v>
+      </c>
       <c r="I19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="J19">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="K19">
+        <v>40.433999999999997</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -1164,9 +1324,22 @@
       <c r="F20" s="14">
         <v>4</v>
       </c>
-      <c r="G20" s="4"/>
+      <c r="G20" s="4">
+        <v>2.9239999999999999</v>
+      </c>
+      <c r="H20">
+        <v>6306</v>
+      </c>
       <c r="I20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="J20">
+        <v>0.108</v>
+      </c>
+      <c r="K20">
+        <v>58.037999999999997</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.35299999999999998</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -1187,9 +1360,22 @@
       <c r="F21" s="14">
         <v>5</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4">
+        <v>10.118</v>
+      </c>
+      <c r="H21">
+        <v>20588</v>
+      </c>
       <c r="I21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="J21">
+        <v>0.106</v>
+      </c>
+      <c r="K21">
+        <v>111.312</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.33500000000000002</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -1210,9 +1396,22 @@
       <c r="F22" s="14">
         <v>6</v>
       </c>
-      <c r="G22" s="4"/>
+      <c r="G22" s="4">
+        <v>43.649000000000001</v>
+      </c>
+      <c r="H22">
+        <v>65230</v>
+      </c>
       <c r="I22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="J22">
+        <v>0.109</v>
+      </c>
+      <c r="K22">
+        <v>20.902999999999999</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.32600000000000001</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -1233,9 +1432,22 @@
       <c r="F23" s="14">
         <v>7</v>
       </c>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4">
+        <v>209.23500000000001</v>
+      </c>
+      <c r="H23">
+        <v>202952</v>
+      </c>
       <c r="I23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="J23">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="K23">
+        <v>232.37299999999999</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0.38</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1262,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936F52FE-6592-4EC8-BB4C-3889BAF1D620}">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="J13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1279,8 +1491,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
-        <v>82</v>
+      <c r="A1" s="29" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -1292,53 +1504,53 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="18" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="24" t="s">
+      <c r="E4" s="23"/>
+      <c r="F4" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="18" t="s">
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="19"/>
-      <c r="M4" s="20"/>
-      <c r="O4" s="20" t="s">
+      <c r="L4" s="22"/>
+      <c r="M4" s="23"/>
+      <c r="O4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="18" t="s">
+      <c r="Q4" s="23"/>
+      <c r="R4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="19"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="18" t="s">
+      <c r="S4" s="22"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="19"/>
-      <c r="W4" s="20"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="23"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
@@ -1351,8 +1563,8 @@
       <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1371,7 +1583,7 @@
       <c r="M5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="21"/>
+      <c r="O5" s="24"/>
       <c r="P5" s="7" t="s">
         <v>18</v>
       </c>
@@ -1398,426 +1610,796 @@
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="14">
-        <v>6</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="J6" s="15"/>
-      <c r="M6" s="1"/>
-      <c r="O6" s="1">
-        <v>1</v>
-      </c>
-      <c r="P6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q6" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="4"/>
-      <c r="T6" s="1"/>
-      <c r="W6" s="1"/>
+      <c r="A6" s="30">
+        <v>0</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="18">
+        <v>28.274000000000001</v>
+      </c>
+      <c r="I6" s="18">
+        <v>110298</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="18">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="L6" s="18">
+        <v>7.8689999999999998</v>
+      </c>
+      <c r="M6" s="16">
+        <v>0.246</v>
+      </c>
+      <c r="O6" s="30">
+        <v>0</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="R6" s="18">
+        <v>28.257999999999999</v>
+      </c>
+      <c r="S6" s="18">
+        <v>110298</v>
+      </c>
+      <c r="T6" s="16"/>
+      <c r="U6" s="18">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="V6" s="18">
+        <v>14.715</v>
+      </c>
+      <c r="W6" s="16">
+        <v>0.26500000000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="G7" s="14">
-        <v>5</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="J7" s="1"/>
-      <c r="M7" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="H7" s="18">
+        <v>36.281999999999996</v>
+      </c>
+      <c r="I7" s="31">
+        <v>112592</v>
+      </c>
+      <c r="J7" s="32"/>
+      <c r="K7" s="31">
+        <v>0.12</v>
+      </c>
+      <c r="L7" s="31">
+        <v>9.4559999999999995</v>
+      </c>
+      <c r="M7" s="16">
+        <v>0.30199999999999999</v>
+      </c>
       <c r="O7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="R7" s="4"/>
-      <c r="T7" s="1"/>
-      <c r="W7" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="R7" s="18">
+        <v>35.768999999999998</v>
+      </c>
+      <c r="S7" s="31">
+        <v>112592</v>
+      </c>
+      <c r="T7" s="16"/>
+      <c r="U7" s="31">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="V7" s="31">
+        <v>12.988</v>
+      </c>
+      <c r="W7" s="16">
+        <v>0.27400000000000002</v>
+      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="14">
-        <v>4</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="J8" s="1"/>
-      <c r="M8" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="H8" s="18">
+        <v>36.756</v>
+      </c>
+      <c r="I8" s="31">
+        <v>113816</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="31">
+        <v>0.108</v>
+      </c>
+      <c r="L8" s="31">
+        <v>8.0109999999999992</v>
+      </c>
+      <c r="M8" s="16">
+        <v>0.26500000000000001</v>
+      </c>
       <c r="O8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P8" s="13" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="R8" s="4"/>
-      <c r="T8" s="1"/>
-      <c r="W8" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="R8" s="18">
+        <v>47.673000000000002</v>
+      </c>
+      <c r="S8" s="31">
+        <v>116118</v>
+      </c>
+      <c r="T8" s="16"/>
+      <c r="U8" s="31">
+        <v>0.105</v>
+      </c>
+      <c r="V8" s="31">
+        <v>9.0790000000000006</v>
+      </c>
+      <c r="W8" s="16">
+        <v>0.28100000000000003</v>
+      </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="14">
         <v>4</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="14">
+      <c r="H9" s="18">
+        <v>36.908000000000001</v>
+      </c>
+      <c r="I9" s="31">
+        <v>115572</v>
+      </c>
+      <c r="J9" s="16"/>
+      <c r="K9" s="31">
+        <v>0.106</v>
+      </c>
+      <c r="L9" s="31">
+        <v>8.0690000000000008</v>
+      </c>
+      <c r="M9" s="16">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="O9" s="1">
         <v>3</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="J9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="O9" s="1">
-        <v>4</v>
-      </c>
       <c r="P9" s="13" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="R9" s="4"/>
-      <c r="T9" s="1"/>
-      <c r="W9" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="R9" s="18">
+        <v>56.835000000000001</v>
+      </c>
+      <c r="S9" s="31">
+        <v>121436</v>
+      </c>
+      <c r="T9" s="16"/>
+      <c r="U9" s="31">
+        <v>0.109</v>
+      </c>
+      <c r="V9" s="31">
+        <v>24.893000000000001</v>
+      </c>
+      <c r="W9" s="16">
+        <v>0.29799999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="14">
-        <v>2</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="J10" s="1"/>
-      <c r="M10" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="H10" s="18">
+        <v>40.856000000000002</v>
+      </c>
+      <c r="I10" s="31">
+        <v>118292</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="31">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="L10" s="31">
+        <v>9.8759999999999994</v>
+      </c>
+      <c r="M10" s="16">
+        <v>0.28199999999999997</v>
+      </c>
       <c r="O10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="R10" s="4"/>
-      <c r="T10" s="1"/>
-      <c r="W10" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="R10" s="18">
+        <v>73.058000000000007</v>
+      </c>
+      <c r="S10" s="31">
+        <v>129590</v>
+      </c>
+      <c r="T10" s="16"/>
+      <c r="U10" s="31">
+        <v>0.11</v>
+      </c>
+      <c r="V10" s="31">
+        <v>30.411999999999999</v>
+      </c>
+      <c r="W10" s="16">
+        <v>0.32500000000000001</v>
+      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" s="14">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="J11" s="15"/>
-      <c r="M11" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="H11" s="18">
+        <v>38.173000000000002</v>
+      </c>
+      <c r="I11" s="31">
+        <v>122652</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="L11" s="31">
+        <v>10.869</v>
+      </c>
+      <c r="M11" s="16">
+        <v>0.26500000000000001</v>
+      </c>
       <c r="O11" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="R11" s="4"/>
-      <c r="T11" s="1"/>
-      <c r="W11" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="R11" s="18">
+        <v>98.23</v>
+      </c>
+      <c r="S11" s="31">
+        <v>142476</v>
+      </c>
+      <c r="T11" s="16"/>
+      <c r="U11" s="31">
+        <v>0.11</v>
+      </c>
+      <c r="V11" s="31">
+        <v>30.675999999999998</v>
+      </c>
+      <c r="W11" s="16">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
+        <v>6</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1</v>
+      </c>
+      <c r="H12" s="18">
+        <v>41.685000000000002</v>
+      </c>
+      <c r="I12" s="31">
+        <v>130076</v>
+      </c>
+      <c r="J12" s="32"/>
+      <c r="K12" s="31">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="L12" s="31">
+        <v>7.6479999999999997</v>
+      </c>
+      <c r="M12" s="16">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="O12" s="1">
+        <v>6</v>
+      </c>
+      <c r="P12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="R12" s="18">
+        <v>136.50299999999999</v>
+      </c>
+      <c r="S12" s="31">
+        <v>163958</v>
+      </c>
+      <c r="T12" s="16"/>
+      <c r="U12" s="31">
+        <v>0.112</v>
+      </c>
+      <c r="V12" s="31">
+        <v>28.869</v>
+      </c>
+      <c r="W12" s="16">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>7</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B13" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C13" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E13" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G13" s="14">
         <v>0</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="J12" s="15"/>
-      <c r="M12" s="1"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="O14" s="2" t="s">
+      <c r="H13" s="18">
+        <v>47.811</v>
+      </c>
+      <c r="I13" s="31">
+        <v>143952</v>
+      </c>
+      <c r="J13" s="32"/>
+      <c r="K13" s="31">
+        <v>0.106</v>
+      </c>
+      <c r="L13" s="31">
+        <v>8.4019999999999992</v>
+      </c>
+      <c r="M13" s="16">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="O13" s="33">
+        <v>7</v>
+      </c>
+      <c r="P13" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="R13" s="18">
+        <v>212.702</v>
+      </c>
+      <c r="S13" s="18">
+        <v>202952</v>
+      </c>
+      <c r="T13" s="16"/>
+      <c r="U13" s="18">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="V13" s="18">
+        <v>165.84800000000001</v>
+      </c>
+      <c r="W13" s="16">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="X13" s="4"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="O15" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="O15" s="20" t="s">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="O16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="18" t="s">
+      <c r="P16" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="18" t="s">
+      <c r="Q16" s="23"/>
+      <c r="R16" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="S15" s="19"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="18" t="s">
+      <c r="S16" s="22"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="V15" s="19"/>
-      <c r="W15" s="20"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="O16" s="21"/>
-      <c r="P16" s="7" t="s">
+      <c r="V16" s="22"/>
+      <c r="W16" s="23"/>
+    </row>
+    <row r="17" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O17" s="24"/>
+      <c r="P17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q16" s="5" t="s">
+      <c r="Q17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="R16" s="7" t="s">
+      <c r="R17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="S16" s="7" t="s">
+      <c r="S17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="T16" s="5" t="s">
+      <c r="T17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="U16" s="7" t="s">
+      <c r="U17" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="V16" s="7" t="s">
+      <c r="V17" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="W16" s="5" t="s">
+      <c r="W17" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O17" s="1">
-        <v>1</v>
-      </c>
-      <c r="P17" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q17" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="R17" s="4"/>
-      <c r="T17" s="1"/>
-      <c r="W17" s="1"/>
-    </row>
     <row r="18" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O18" s="1">
-        <v>2</v>
-      </c>
-      <c r="P18" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q18" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="R18" s="4"/>
-      <c r="T18" s="1"/>
-      <c r="W18" s="1"/>
+      <c r="O18" s="30">
+        <v>0</v>
+      </c>
+      <c r="P18" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q18" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="R18" s="18">
+        <v>27.352</v>
+      </c>
+      <c r="S18" s="18">
+        <v>110298</v>
+      </c>
+      <c r="T18" s="16"/>
+      <c r="U18" s="18">
+        <v>0.124</v>
+      </c>
+      <c r="V18" s="18">
+        <v>7.91</v>
+      </c>
+      <c r="W18" s="16">
+        <v>0.29299999999999998</v>
+      </c>
     </row>
     <row r="19" spans="15:24" x14ac:dyDescent="0.3">
       <c r="O19" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="Q19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="R19" s="4"/>
-      <c r="T19" s="1"/>
-      <c r="W19" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="R19" s="18">
+        <v>44.231999999999999</v>
+      </c>
+      <c r="S19" s="31">
+        <v>143952</v>
+      </c>
+      <c r="T19" s="16"/>
+      <c r="U19" s="31">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="V19" s="31">
+        <v>9.7370000000000001</v>
+      </c>
+      <c r="W19" s="16">
+        <v>0.26600000000000001</v>
+      </c>
     </row>
     <row r="20" spans="15:24" x14ac:dyDescent="0.3">
       <c r="O20" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P20" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q20" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="R20" s="4"/>
-      <c r="T20" s="1"/>
-      <c r="W20" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="R20" s="18">
+        <v>67.411000000000001</v>
+      </c>
+      <c r="S20" s="31">
+        <v>165678</v>
+      </c>
+      <c r="T20" s="16"/>
+      <c r="U20" s="31">
+        <v>0.104</v>
+      </c>
+      <c r="V20" s="31">
+        <v>19.459</v>
+      </c>
+      <c r="W20" s="16">
+        <v>0.28699999999999998</v>
+      </c>
     </row>
     <row r="21" spans="15:24" x14ac:dyDescent="0.3">
       <c r="O21" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="Q21" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="R21" s="4"/>
-      <c r="T21" s="1"/>
-      <c r="W21" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="R21" s="18">
+        <v>87.522999999999996</v>
+      </c>
+      <c r="S21" s="31">
+        <v>179984</v>
+      </c>
+      <c r="T21" s="16"/>
+      <c r="U21" s="31">
+        <v>0.105</v>
+      </c>
+      <c r="V21" s="31">
+        <v>10.725</v>
+      </c>
+      <c r="W21" s="16">
+        <v>0.32600000000000001</v>
+      </c>
     </row>
     <row r="22" spans="15:24" x14ac:dyDescent="0.3">
       <c r="O22" s="1">
+        <v>4</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q22" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="R22" s="18">
+        <v>116.637</v>
+      </c>
+      <c r="S22" s="31">
+        <v>189502</v>
+      </c>
+      <c r="T22" s="16"/>
+      <c r="U22" s="31">
+        <v>0.107</v>
+      </c>
+      <c r="V22" s="31">
+        <v>19.972999999999999</v>
+      </c>
+      <c r="W22" s="16">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="23" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O23" s="1">
+        <v>5</v>
+      </c>
+      <c r="P23" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q23" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="R23" s="18">
+        <v>149.12</v>
+      </c>
+      <c r="S23" s="31">
+        <v>195872</v>
+      </c>
+      <c r="T23" s="16"/>
+      <c r="U23" s="31">
+        <v>0.112</v>
+      </c>
+      <c r="V23" s="31">
+        <v>18.366</v>
+      </c>
+      <c r="W23" s="16">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="24" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O24" s="1">
         <v>6</v>
       </c>
-      <c r="P22" s="13" t="s">
+      <c r="P24" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="Q22" s="11" t="s">
+      <c r="Q24" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="R22" s="4"/>
-      <c r="T22" s="1"/>
-      <c r="W22" s="1"/>
-    </row>
-    <row r="23" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O23" s="4"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
+      <c r="R24" s="18">
+        <v>182.76400000000001</v>
+      </c>
+      <c r="S24" s="31">
+        <v>200154</v>
+      </c>
+      <c r="T24" s="16"/>
+      <c r="U24" s="31">
+        <v>0.113</v>
+      </c>
+      <c r="V24" s="31">
+        <v>14.159000000000001</v>
+      </c>
+      <c r="W24" s="16">
+        <v>0.36699999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O25" s="33">
+        <v>7</v>
+      </c>
+      <c r="P25" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q25" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="R25" s="18">
+        <v>224.78</v>
+      </c>
+      <c r="S25" s="18">
+        <v>202952</v>
+      </c>
+      <c r="T25" s="16"/>
+      <c r="U25" s="18">
+        <v>0.156</v>
+      </c>
+      <c r="V25" s="18">
+        <v>166.749</v>
+      </c>
+      <c r="W25" s="16">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="X25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
     <mergeCell ref="R4:T4"/>
     <mergeCell ref="U4:W4"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="O16:O17"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="A4:A5"/>
@@ -1830,18 +2412,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F6:F12" numberStoredAsText="1"/>
-    <ignoredError sqref="C10:C11 E6:E8" twoDigitTextYear="1"/>
+    <ignoredError sqref="F7:F13" numberStoredAsText="1"/>
+    <ignoredError sqref="C11:C12 E7:E9" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7664E89F-51BA-4878-9967-5F93A0459797}">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23:V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1854,8 +2436,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
-        <v>82</v>
+      <c r="A1" s="29" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
@@ -1867,52 +2449,52 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="18" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="24" t="s">
+      <c r="E4" s="23"/>
+      <c r="F4" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="18" t="s">
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="19"/>
-      <c r="M4" s="20"/>
-      <c r="O4" s="20" t="s">
+      <c r="L4" s="22"/>
+      <c r="M4" s="23"/>
+      <c r="O4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="18" t="s">
+      <c r="Q4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="19"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="18" t="s">
+      <c r="R4" s="22"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="19"/>
-      <c r="V4" s="20"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="23"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
@@ -1925,8 +2507,8 @@
       <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1945,8 +2527,8 @@
       <c r="M5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="21"/>
-      <c r="P5" s="25"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="28"/>
       <c r="Q5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1967,332 +2549,651 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="14">
-        <v>6</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="J6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="O6" s="1">
-        <v>1</v>
-      </c>
-      <c r="P6" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="4"/>
-      <c r="S6" s="1"/>
-      <c r="V6" s="1"/>
+      <c r="A6" s="30">
+        <v>0</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="18">
+        <v>27.649000000000001</v>
+      </c>
+      <c r="I6" s="18">
+        <v>110298</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="18">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="L6" s="18">
+        <v>9.4469999999999992</v>
+      </c>
+      <c r="M6" s="16">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="O6" s="30">
+        <v>0</v>
+      </c>
+      <c r="P6" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>27.878</v>
+      </c>
+      <c r="R6" s="18">
+        <v>110298</v>
+      </c>
+      <c r="S6" s="16"/>
+      <c r="T6" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="U6" s="18">
+        <v>7.6459999999999999</v>
+      </c>
+      <c r="V6" s="16">
+        <v>0.254</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="14">
-        <v>5</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="J7" s="1"/>
-      <c r="M7" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="H7" s="18">
+        <v>28.402999999999999</v>
+      </c>
+      <c r="I7" s="31">
+        <v>107463</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="31">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="L7" s="31">
+        <v>9.8040000000000003</v>
+      </c>
+      <c r="M7" s="16">
+        <v>0.255</v>
+      </c>
       <c r="O7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7" s="14">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="4"/>
-      <c r="S7" s="1"/>
-      <c r="V7" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q7" s="18">
+        <v>28.166</v>
+      </c>
+      <c r="R7" s="31">
+        <v>107463</v>
+      </c>
+      <c r="S7" s="16"/>
+      <c r="T7" s="31">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="U7" s="31">
+        <v>61.7</v>
+      </c>
+      <c r="V7" s="16">
+        <v>0.25900000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="G8" s="14">
-        <v>4</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="J8" s="1"/>
-      <c r="M8" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="H8" s="18">
+        <v>26.989000000000001</v>
+      </c>
+      <c r="I8" s="31">
+        <v>102891</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="31">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="L8" s="31">
+        <v>9.3350000000000009</v>
+      </c>
+      <c r="M8" s="16">
+        <v>0.25700000000000001</v>
+      </c>
       <c r="O8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P8" s="14">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="4"/>
-      <c r="S8" s="1"/>
-      <c r="V8" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>28.323</v>
+      </c>
+      <c r="R8" s="31">
+        <v>103228</v>
+      </c>
+      <c r="S8" s="16"/>
+      <c r="T8" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="U8" s="31">
+        <v>8.6059999999999999</v>
+      </c>
+      <c r="V8" s="16">
+        <v>0.249</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="14">
         <v>4</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="14">
+      <c r="H9" s="18">
+        <v>24.521999999999998</v>
+      </c>
+      <c r="I9" s="31">
+        <v>96521</v>
+      </c>
+      <c r="J9" s="16"/>
+      <c r="K9" s="31">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="L9" s="31">
+        <v>7.9829999999999997</v>
+      </c>
+      <c r="M9" s="16">
+        <v>0.248</v>
+      </c>
+      <c r="O9" s="1">
         <v>3</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="J9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="O9" s="1">
-        <v>4</v>
-      </c>
       <c r="P9" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q9" s="4"/>
-      <c r="S9" s="1"/>
-      <c r="V9" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>27.428000000000001</v>
+      </c>
+      <c r="R9" s="31">
+        <v>97173</v>
+      </c>
+      <c r="S9" s="16"/>
+      <c r="T9" s="31">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="U9" s="31">
+        <v>10.391</v>
+      </c>
+      <c r="V9" s="16">
+        <v>0.25600000000000001</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" s="14">
-        <v>2</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="J10" s="1"/>
-      <c r="M10" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="H10" s="18">
+        <v>22.553000000000001</v>
+      </c>
+      <c r="I10" s="31">
+        <v>88323</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="31">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="L10" s="31">
+        <v>7.9669999999999996</v>
+      </c>
+      <c r="M10" s="16">
+        <v>0.248</v>
+      </c>
       <c r="O10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P10" s="14">
-        <v>5</v>
-      </c>
-      <c r="Q10" s="4"/>
-      <c r="S10" s="1"/>
-      <c r="V10" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q10" s="18">
+        <v>25.245000000000001</v>
+      </c>
+      <c r="R10" s="31">
+        <v>88866</v>
+      </c>
+      <c r="S10" s="16"/>
+      <c r="T10" s="31">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="U10" s="31">
+        <v>10.505000000000001</v>
+      </c>
+      <c r="V10" s="16">
+        <v>0.248</v>
+      </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
+        <v>5</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="14">
+        <v>2</v>
+      </c>
+      <c r="H11" s="18">
+        <v>20.119</v>
+      </c>
+      <c r="I11" s="31">
+        <v>80073</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="31">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="L11" s="31">
+        <v>17.106999999999999</v>
+      </c>
+      <c r="M11" s="16">
+        <v>0.254</v>
+      </c>
+      <c r="O11" s="1">
+        <v>5</v>
+      </c>
+      <c r="P11" s="14">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="18">
+        <v>22.638000000000002</v>
+      </c>
+      <c r="R11" s="31">
+        <v>78631</v>
+      </c>
+      <c r="S11" s="16"/>
+      <c r="T11" s="31">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="U11" s="31">
+        <v>16.93</v>
+      </c>
+      <c r="V11" s="16">
+        <v>0.27900000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>6</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F12" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G12" s="14">
         <v>1</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="J11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="O11" s="1">
+      <c r="H12" s="18">
+        <v>18.905000000000001</v>
+      </c>
+      <c r="I12" s="31">
+        <v>79949</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="31">
+        <v>9.4E-2</v>
+      </c>
+      <c r="L12" s="31">
+        <v>8.6319999999999997</v>
+      </c>
+      <c r="M12" s="16">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="O12" s="1">
         <v>6</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P12" s="14">
         <v>6</v>
       </c>
-      <c r="Q11" s="4"/>
-      <c r="S11" s="1"/>
-      <c r="V11" s="1"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O13" s="2" t="s">
+      <c r="Q12" s="18">
+        <v>21.321000000000002</v>
+      </c>
+      <c r="R12" s="31">
+        <v>69870</v>
+      </c>
+      <c r="S12" s="16"/>
+      <c r="T12" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="U12" s="31">
+        <v>8.7430000000000003</v>
+      </c>
+      <c r="V12" s="16">
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="O14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O14" s="20" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="O15" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="P14" s="24" t="s">
+      <c r="P15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="Q14" s="18" t="s">
+      <c r="Q15" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="R14" s="19"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="18" t="s">
+      <c r="R15" s="22"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="U14" s="19"/>
-      <c r="V14" s="20"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O15" s="21"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="7" t="s">
+      <c r="U15" s="22"/>
+      <c r="V15" s="23"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="O16" s="24"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="R15" s="7" t="s">
+      <c r="R16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="S15" s="5" t="s">
+      <c r="S16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="T15" s="7" t="s">
+      <c r="T16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="U15" s="7" t="s">
+      <c r="U16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="V15" s="5" t="s">
+      <c r="V16" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O16" s="1">
-        <v>1</v>
-      </c>
-      <c r="P16" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="4"/>
-      <c r="S16" s="1"/>
-      <c r="V16" s="1"/>
-    </row>
     <row r="17" spans="15:22" x14ac:dyDescent="0.3">
-      <c r="O17" s="1">
-        <v>2</v>
-      </c>
-      <c r="P17" s="14">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="4"/>
-      <c r="S17" s="1"/>
-      <c r="V17" s="1"/>
+      <c r="O17" s="30">
+        <v>0</v>
+      </c>
+      <c r="P17" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="18">
+        <v>27.527000000000001</v>
+      </c>
+      <c r="R17" s="18">
+        <v>110298</v>
+      </c>
+      <c r="S17" s="16"/>
+      <c r="T17" s="18">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="U17" s="18">
+        <v>8.8580000000000005</v>
+      </c>
+      <c r="V17" s="16">
+        <v>0.249</v>
+      </c>
     </row>
     <row r="18" spans="15:22" x14ac:dyDescent="0.3">
       <c r="O18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P18" s="14">
-        <v>3</v>
-      </c>
-      <c r="Q18" s="4"/>
-      <c r="S18" s="1"/>
-      <c r="V18" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q18" s="18">
+        <v>20.341000000000001</v>
+      </c>
+      <c r="R18" s="31">
+        <v>79949</v>
+      </c>
+      <c r="S18" s="16"/>
+      <c r="T18" s="31">
+        <v>0.109</v>
+      </c>
+      <c r="U18" s="31">
+        <v>9.3439999999999994</v>
+      </c>
+      <c r="V18" s="16">
+        <v>0.27100000000000002</v>
+      </c>
     </row>
     <row r="19" spans="15:22" x14ac:dyDescent="0.3">
       <c r="O19" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P19" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q19" s="4"/>
-      <c r="S19" s="1"/>
-      <c r="V19" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q19" s="18">
+        <v>17.306999999999999</v>
+      </c>
+      <c r="R19" s="31">
+        <v>71312</v>
+      </c>
+      <c r="S19" s="16"/>
+      <c r="T19" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="U19" s="31">
+        <v>15.314</v>
+      </c>
+      <c r="V19" s="16">
+        <v>0.26600000000000001</v>
+      </c>
     </row>
     <row r="20" spans="15:22" x14ac:dyDescent="0.3">
       <c r="O20" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P20" s="14">
-        <v>5</v>
-      </c>
-      <c r="Q20" s="4"/>
-      <c r="S20" s="1"/>
-      <c r="V20" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q20" s="18">
+        <v>17.437999999999999</v>
+      </c>
+      <c r="R20" s="31">
+        <v>69327</v>
+      </c>
+      <c r="S20" s="16"/>
+      <c r="T20" s="31">
+        <v>0.09</v>
+      </c>
+      <c r="U20" s="31">
+        <v>11.083</v>
+      </c>
+      <c r="V20" s="16">
+        <v>0.252</v>
+      </c>
     </row>
     <row r="21" spans="15:22" x14ac:dyDescent="0.3">
       <c r="O21" s="1">
+        <v>4</v>
+      </c>
+      <c r="P21" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="18">
+        <v>17.946999999999999</v>
+      </c>
+      <c r="R21" s="31">
+        <v>69218</v>
+      </c>
+      <c r="S21" s="16"/>
+      <c r="T21" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="U21" s="31">
+        <v>13.476000000000001</v>
+      </c>
+      <c r="V21" s="16">
+        <v>0.247</v>
+      </c>
+    </row>
+    <row r="22" spans="15:22" x14ac:dyDescent="0.3">
+      <c r="O22" s="1">
+        <v>5</v>
+      </c>
+      <c r="P22" s="14">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="18">
+        <v>18.53</v>
+      </c>
+      <c r="R22" s="31">
+        <v>69533</v>
+      </c>
+      <c r="S22" s="16"/>
+      <c r="T22" s="31">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="U22" s="31">
+        <v>8.2609999999999992</v>
+      </c>
+      <c r="V22" s="16">
+        <v>0.24099999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="15:22" x14ac:dyDescent="0.3">
+      <c r="O23" s="1">
         <v>6</v>
       </c>
-      <c r="P21" s="14">
+      <c r="P23" s="14">
         <v>6</v>
       </c>
-      <c r="Q21" s="4"/>
-      <c r="S21" s="1"/>
-      <c r="V21" s="1"/>
+      <c r="Q23" s="18">
+        <v>20.381</v>
+      </c>
+      <c r="R23" s="31">
+        <v>69870</v>
+      </c>
+      <c r="S23" s="16"/>
+      <c r="T23" s="31">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="U23" s="31">
+        <v>14.048999999999999</v>
+      </c>
+      <c r="V23" s="16">
+        <v>0.246</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="T4:V4"/>
-    <mergeCell ref="Q14:S14"/>
-    <mergeCell ref="T14:V14"/>
-    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="T15:V15"/>
+    <mergeCell ref="O15:O16"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -2302,13 +3203,13 @@
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:P5"/>
-    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="P15:P16"/>
     <mergeCell ref="Q4:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="C9:C10 E7:E8" twoDigitTextYear="1"/>
-    <ignoredError sqref="F6 F7:F11" numberStoredAsText="1"/>
+    <ignoredError sqref="C10:C11 E8:E9" twoDigitTextYear="1"/>
+    <ignoredError sqref="F7 F8:F12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Indicative memory usage for the first two tests
</commit_message>
<xml_diff>
--- a/input/core_algorithms_2022/Experiment_results.xlsx
+++ b/input/core_algorithms_2022/Experiment_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_Devel\Repos\repos-2020-06\model-interplay-monitoring-code\input\core_algorithms_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD95F099-6B2E-4818-BA07-559557704DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1548674-ECC7-4459-A256-0703499919E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="2400" windowWidth="20760" windowHeight="11505" activeTab="2" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
+    <workbookView xWindow="-3945" yWindow="-21720" windowWidth="38640" windowHeight="21390" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
   </bookViews>
   <sheets>
     <sheet name="modelSize" sheetId="6" r:id="rId1"/>
@@ -284,16 +284,16 @@
     <t>Number of guards (end -&gt; beginning)</t>
   </si>
   <si>
-    <t>NB! The non-deterministic nature of Java GC means that memory consumption with the same inputs may vary significantly (up to multiple GB in some tests).</t>
-  </si>
-  <si>
-    <t>NB! The non-deterministic nature of Java GC means that memory consumption with the same inputs may vary significantly (up to multiple GB in some tests) and is therefore currently not measured.</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>14/7</t>
+  </si>
+  <si>
+    <t>NB! The non-deterministic nature of Java GC means that memory consumption with the same inputs may vary significantly (up to multiple GB in some tests) and is not measured here.</t>
+  </si>
+  <si>
+    <t>NB! The non-deterministic nature of Java GC means that memory consumption with the same inputs may vary significantly (up to multiple GB in some tests), values given here should be seen as indicative of the overal trend only.</t>
   </si>
 </sst>
 </file>
@@ -500,6 +500,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -524,17 +535,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D70222-B554-4BB9-8CB5-22FD4E14CBB3}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23:L23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -863,8 +863,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>82</v>
+      <c r="A1" s="21" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -873,36 +873,36 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="27" t="s">
+      <c r="C4" s="31"/>
+      <c r="D4" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="21" t="s">
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="28"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="28"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
@@ -941,7 +941,9 @@
       <c r="F6">
         <v>54</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3">
+        <v>182</v>
+      </c>
       <c r="H6">
         <v>9.4E-2</v>
       </c>
@@ -971,7 +973,9 @@
       <c r="F7">
         <v>272</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>185</v>
+      </c>
       <c r="H7">
         <v>9.9000000000000005E-2</v>
       </c>
@@ -1001,7 +1005,9 @@
       <c r="F8">
         <v>1026</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>197</v>
+      </c>
       <c r="H8">
         <v>0.115</v>
       </c>
@@ -1031,7 +1037,9 @@
       <c r="F9">
         <v>3484</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>229</v>
+      </c>
       <c r="H9">
         <v>0.111</v>
       </c>
@@ -1061,7 +1069,9 @@
       <c r="F10">
         <v>11278</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1">
+        <v>517</v>
+      </c>
       <c r="H10">
         <v>0.10100000000000001</v>
       </c>
@@ -1091,7 +1101,9 @@
       <c r="F11">
         <v>35560</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <v>1450</v>
+      </c>
       <c r="H11">
         <v>0.10199999999999999</v>
       </c>
@@ -1121,7 +1133,9 @@
       <c r="F12">
         <v>110298</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <v>5047</v>
+      </c>
       <c r="H12">
         <v>9.9000000000000005E-2</v>
       </c>
@@ -1138,33 +1152,33 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="21" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="27" t="s">
+      <c r="E15" s="28"/>
+      <c r="F15" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="21" t="s">
+      <c r="H15" s="27"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="22"/>
-      <c r="L15" s="23"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="28"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
@@ -1177,7 +1191,7 @@
       <c r="E16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="28"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="7" t="s">
         <v>12</v>
       </c>
@@ -1222,7 +1236,9 @@
       <c r="H17">
         <v>80</v>
       </c>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3">
+        <v>184</v>
+      </c>
       <c r="J17">
         <v>0.10299999999999999</v>
       </c>
@@ -1258,7 +1274,9 @@
       <c r="H18">
         <v>462</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="1">
+        <v>195</v>
+      </c>
       <c r="J18">
         <v>0.10299999999999999</v>
       </c>
@@ -1294,7 +1312,9 @@
       <c r="H19">
         <v>1824</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1">
+        <v>233</v>
+      </c>
       <c r="J19">
         <v>9.5000000000000001E-2</v>
       </c>
@@ -1330,7 +1350,9 @@
       <c r="H20">
         <v>6306</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1">
+        <v>545</v>
+      </c>
       <c r="J20">
         <v>0.108</v>
       </c>
@@ -1366,7 +1388,9 @@
       <c r="H21">
         <v>20588</v>
       </c>
-      <c r="I21" s="1"/>
+      <c r="I21" s="1">
+        <v>1308</v>
+      </c>
       <c r="J21">
         <v>0.106</v>
       </c>
@@ -1402,7 +1426,9 @@
       <c r="H22">
         <v>65230</v>
       </c>
-      <c r="I22" s="1"/>
+      <c r="I22" s="1">
+        <v>4829</v>
+      </c>
       <c r="J22">
         <v>0.109</v>
       </c>
@@ -1438,7 +1464,9 @@
       <c r="H23">
         <v>202952</v>
       </c>
-      <c r="I23" s="1"/>
+      <c r="I23" s="1">
+        <v>13975</v>
+      </c>
       <c r="J23">
         <v>0.11600000000000001</v>
       </c>
@@ -1476,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936F52FE-6592-4EC8-BB4C-3889BAF1D620}">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView topLeftCell="J13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1491,8 +1519,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>83</v>
+      <c r="A1" s="21" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -1504,53 +1532,53 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="27" t="s">
+      <c r="E4" s="28"/>
+      <c r="F4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="21" t="s">
+      <c r="I4" s="27"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="22"/>
-      <c r="M4" s="23"/>
-      <c r="O4" s="23" t="s">
+      <c r="L4" s="27"/>
+      <c r="M4" s="28"/>
+      <c r="O4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="P4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="21" t="s">
+      <c r="Q4" s="28"/>
+      <c r="R4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="22"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="21" t="s">
+      <c r="S4" s="27"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="22"/>
-      <c r="W4" s="23"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="28"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
@@ -1563,8 +1591,8 @@
       <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1583,7 +1611,7 @@
       <c r="M5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="24"/>
+      <c r="O5" s="29"/>
       <c r="P5" s="7" t="s">
         <v>18</v>
       </c>
@@ -1610,26 +1638,26 @@
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="22">
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H6" s="18">
         <v>28.274000000000001</v>
@@ -1647,7 +1675,7 @@
       <c r="M6" s="16">
         <v>0.246</v>
       </c>
-      <c r="O6" s="30">
+      <c r="O6" s="22">
         <v>0</v>
       </c>
       <c r="P6" s="18" t="s">
@@ -1698,14 +1726,14 @@
       <c r="H7" s="18">
         <v>36.281999999999996</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="23">
         <v>112592</v>
       </c>
-      <c r="J7" s="32"/>
-      <c r="K7" s="31">
+      <c r="J7" s="24"/>
+      <c r="K7" s="23">
         <v>0.12</v>
       </c>
-      <c r="L7" s="31">
+      <c r="L7" s="23">
         <v>9.4559999999999995</v>
       </c>
       <c r="M7" s="16">
@@ -1723,14 +1751,14 @@
       <c r="R7" s="18">
         <v>35.768999999999998</v>
       </c>
-      <c r="S7" s="31">
+      <c r="S7" s="23">
         <v>112592</v>
       </c>
       <c r="T7" s="16"/>
-      <c r="U7" s="31">
+      <c r="U7" s="23">
         <v>0.10299999999999999</v>
       </c>
-      <c r="V7" s="31">
+      <c r="V7" s="23">
         <v>12.988</v>
       </c>
       <c r="W7" s="16">
@@ -1762,14 +1790,14 @@
       <c r="H8" s="18">
         <v>36.756</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="23">
         <v>113816</v>
       </c>
       <c r="J8" s="16"/>
-      <c r="K8" s="31">
+      <c r="K8" s="23">
         <v>0.108</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="23">
         <v>8.0109999999999992</v>
       </c>
       <c r="M8" s="16">
@@ -1787,14 +1815,14 @@
       <c r="R8" s="18">
         <v>47.673000000000002</v>
       </c>
-      <c r="S8" s="31">
+      <c r="S8" s="23">
         <v>116118</v>
       </c>
       <c r="T8" s="16"/>
-      <c r="U8" s="31">
+      <c r="U8" s="23">
         <v>0.105</v>
       </c>
-      <c r="V8" s="31">
+      <c r="V8" s="23">
         <v>9.0790000000000006</v>
       </c>
       <c r="W8" s="16">
@@ -1826,14 +1854,14 @@
       <c r="H9" s="18">
         <v>36.908000000000001</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="23">
         <v>115572</v>
       </c>
       <c r="J9" s="16"/>
-      <c r="K9" s="31">
+      <c r="K9" s="23">
         <v>0.106</v>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="23">
         <v>8.0690000000000008</v>
       </c>
       <c r="M9" s="16">
@@ -1851,14 +1879,14 @@
       <c r="R9" s="18">
         <v>56.835000000000001</v>
       </c>
-      <c r="S9" s="31">
+      <c r="S9" s="23">
         <v>121436</v>
       </c>
       <c r="T9" s="16"/>
-      <c r="U9" s="31">
+      <c r="U9" s="23">
         <v>0.109</v>
       </c>
-      <c r="V9" s="31">
+      <c r="V9" s="23">
         <v>24.893000000000001</v>
       </c>
       <c r="W9" s="16">
@@ -1890,14 +1918,14 @@
       <c r="H10" s="18">
         <v>40.856000000000002</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="23">
         <v>118292</v>
       </c>
       <c r="J10" s="16"/>
-      <c r="K10" s="31">
+      <c r="K10" s="23">
         <v>0.10199999999999999</v>
       </c>
-      <c r="L10" s="31">
+      <c r="L10" s="23">
         <v>9.8759999999999994</v>
       </c>
       <c r="M10" s="16">
@@ -1915,14 +1943,14 @@
       <c r="R10" s="18">
         <v>73.058000000000007</v>
       </c>
-      <c r="S10" s="31">
+      <c r="S10" s="23">
         <v>129590</v>
       </c>
       <c r="T10" s="16"/>
-      <c r="U10" s="31">
+      <c r="U10" s="23">
         <v>0.11</v>
       </c>
-      <c r="V10" s="31">
+      <c r="V10" s="23">
         <v>30.411999999999999</v>
       </c>
       <c r="W10" s="16">
@@ -1954,14 +1982,14 @@
       <c r="H11" s="18">
         <v>38.173000000000002</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I11" s="23">
         <v>122652</v>
       </c>
       <c r="J11" s="16"/>
-      <c r="K11" s="31">
+      <c r="K11" s="23">
         <v>0.1</v>
       </c>
-      <c r="L11" s="31">
+      <c r="L11" s="23">
         <v>10.869</v>
       </c>
       <c r="M11" s="16">
@@ -1979,14 +2007,14 @@
       <c r="R11" s="18">
         <v>98.23</v>
       </c>
-      <c r="S11" s="31">
+      <c r="S11" s="23">
         <v>142476</v>
       </c>
       <c r="T11" s="16"/>
-      <c r="U11" s="31">
+      <c r="U11" s="23">
         <v>0.11</v>
       </c>
-      <c r="V11" s="31">
+      <c r="V11" s="23">
         <v>30.675999999999998</v>
       </c>
       <c r="W11" s="16">
@@ -2018,14 +2046,14 @@
       <c r="H12" s="18">
         <v>41.685000000000002</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="23">
         <v>130076</v>
       </c>
-      <c r="J12" s="32"/>
-      <c r="K12" s="31">
+      <c r="J12" s="24"/>
+      <c r="K12" s="23">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="L12" s="31">
+      <c r="L12" s="23">
         <v>7.6479999999999997</v>
       </c>
       <c r="M12" s="16">
@@ -2043,14 +2071,14 @@
       <c r="R12" s="18">
         <v>136.50299999999999</v>
       </c>
-      <c r="S12" s="31">
+      <c r="S12" s="23">
         <v>163958</v>
       </c>
       <c r="T12" s="16"/>
-      <c r="U12" s="31">
+      <c r="U12" s="23">
         <v>0.112</v>
       </c>
-      <c r="V12" s="31">
+      <c r="V12" s="23">
         <v>28.869</v>
       </c>
       <c r="W12" s="16">
@@ -2082,24 +2110,24 @@
       <c r="H13" s="18">
         <v>47.811</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="23">
         <v>143952</v>
       </c>
-      <c r="J13" s="32"/>
-      <c r="K13" s="31">
+      <c r="J13" s="24"/>
+      <c r="K13" s="23">
         <v>0.106</v>
       </c>
-      <c r="L13" s="31">
+      <c r="L13" s="23">
         <v>8.4019999999999992</v>
       </c>
       <c r="M13" s="16">
         <v>0.26900000000000002</v>
       </c>
-      <c r="O13" s="33">
+      <c r="O13" s="25">
         <v>7</v>
       </c>
       <c r="P13" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q13" s="11" t="s">
         <v>37</v>
@@ -2128,26 +2156,26 @@
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="O16" s="23" t="s">
+      <c r="O16" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="P16" s="21" t="s">
+      <c r="P16" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="21" t="s">
+      <c r="Q16" s="28"/>
+      <c r="R16" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="S16" s="22"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="21" t="s">
+      <c r="S16" s="27"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="V16" s="22"/>
-      <c r="W16" s="23"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="28"/>
     </row>
     <row r="17" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O17" s="24"/>
+      <c r="O17" s="29"/>
       <c r="P17" s="7" t="s">
         <v>18</v>
       </c>
@@ -2174,7 +2202,7 @@
       </c>
     </row>
     <row r="18" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O18" s="30">
+      <c r="O18" s="22">
         <v>0</v>
       </c>
       <c r="P18" s="18" t="s">
@@ -2213,14 +2241,14 @@
       <c r="R19" s="18">
         <v>44.231999999999999</v>
       </c>
-      <c r="S19" s="31">
+      <c r="S19" s="23">
         <v>143952</v>
       </c>
       <c r="T19" s="16"/>
-      <c r="U19" s="31">
+      <c r="U19" s="23">
         <v>0.10100000000000001</v>
       </c>
-      <c r="V19" s="31">
+      <c r="V19" s="23">
         <v>9.7370000000000001</v>
       </c>
       <c r="W19" s="16">
@@ -2240,14 +2268,14 @@
       <c r="R20" s="18">
         <v>67.411000000000001</v>
       </c>
-      <c r="S20" s="31">
+      <c r="S20" s="23">
         <v>165678</v>
       </c>
       <c r="T20" s="16"/>
-      <c r="U20" s="31">
+      <c r="U20" s="23">
         <v>0.104</v>
       </c>
-      <c r="V20" s="31">
+      <c r="V20" s="23">
         <v>19.459</v>
       </c>
       <c r="W20" s="16">
@@ -2267,14 +2295,14 @@
       <c r="R21" s="18">
         <v>87.522999999999996</v>
       </c>
-      <c r="S21" s="31">
+      <c r="S21" s="23">
         <v>179984</v>
       </c>
       <c r="T21" s="16"/>
-      <c r="U21" s="31">
+      <c r="U21" s="23">
         <v>0.105</v>
       </c>
-      <c r="V21" s="31">
+      <c r="V21" s="23">
         <v>10.725</v>
       </c>
       <c r="W21" s="16">
@@ -2294,14 +2322,14 @@
       <c r="R22" s="18">
         <v>116.637</v>
       </c>
-      <c r="S22" s="31">
+      <c r="S22" s="23">
         <v>189502</v>
       </c>
       <c r="T22" s="16"/>
-      <c r="U22" s="31">
+      <c r="U22" s="23">
         <v>0.107</v>
       </c>
-      <c r="V22" s="31">
+      <c r="V22" s="23">
         <v>19.972999999999999</v>
       </c>
       <c r="W22" s="16">
@@ -2321,14 +2349,14 @@
       <c r="R23" s="18">
         <v>149.12</v>
       </c>
-      <c r="S23" s="31">
+      <c r="S23" s="23">
         <v>195872</v>
       </c>
       <c r="T23" s="16"/>
-      <c r="U23" s="31">
+      <c r="U23" s="23">
         <v>0.112</v>
       </c>
-      <c r="V23" s="31">
+      <c r="V23" s="23">
         <v>18.366</v>
       </c>
       <c r="W23" s="16">
@@ -2348,14 +2376,14 @@
       <c r="R24" s="18">
         <v>182.76400000000001</v>
       </c>
-      <c r="S24" s="31">
+      <c r="S24" s="23">
         <v>200154</v>
       </c>
       <c r="T24" s="16"/>
-      <c r="U24" s="31">
+      <c r="U24" s="23">
         <v>0.113</v>
       </c>
-      <c r="V24" s="31">
+      <c r="V24" s="23">
         <v>14.159000000000001</v>
       </c>
       <c r="W24" s="16">
@@ -2363,11 +2391,11 @@
       </c>
     </row>
     <row r="25" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O25" s="33">
+      <c r="O25" s="25">
         <v>7</v>
       </c>
       <c r="P25" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q25" s="11" t="s">
         <v>37</v>
@@ -2392,6 +2420,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="P16:Q16"/>
@@ -2400,13 +2435,6 @@
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="U16:W16"/>
     <mergeCell ref="O16:O17"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2422,8 +2450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7664E89F-51BA-4878-9967-5F93A0459797}">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23:V23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2436,8 +2464,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>83</v>
+      <c r="A1" s="21" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
@@ -2449,52 +2477,52 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="27" t="s">
+      <c r="E4" s="28"/>
+      <c r="F4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="21" t="s">
+      <c r="I4" s="27"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="22"/>
-      <c r="M4" s="23"/>
-      <c r="O4" s="23" t="s">
+      <c r="L4" s="27"/>
+      <c r="M4" s="28"/>
+      <c r="O4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="22"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="21" t="s">
+      <c r="R4" s="27"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="22"/>
-      <c r="V4" s="23"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="28"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
@@ -2507,8 +2535,8 @@
       <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2527,8 +2555,8 @@
       <c r="M5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="24"/>
-      <c r="P5" s="28"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="33"/>
       <c r="Q5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2549,26 +2577,26 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="22">
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H6" s="18">
         <v>27.649000000000001</v>
@@ -2586,7 +2614,7 @@
       <c r="M6" s="16">
         <v>0.26200000000000001</v>
       </c>
-      <c r="O6" s="30">
+      <c r="O6" s="22">
         <v>0</v>
       </c>
       <c r="P6" s="17">
@@ -2634,14 +2662,14 @@
       <c r="H7" s="18">
         <v>28.402999999999999</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="23">
         <v>107463</v>
       </c>
       <c r="J7" s="16"/>
-      <c r="K7" s="31">
+      <c r="K7" s="23">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="L7" s="31">
+      <c r="L7" s="23">
         <v>9.8040000000000003</v>
       </c>
       <c r="M7" s="16">
@@ -2656,14 +2684,14 @@
       <c r="Q7" s="18">
         <v>28.166</v>
       </c>
-      <c r="R7" s="31">
+      <c r="R7" s="23">
         <v>107463</v>
       </c>
       <c r="S7" s="16"/>
-      <c r="T7" s="31">
+      <c r="T7" s="23">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="U7" s="31">
+      <c r="U7" s="23">
         <v>61.7</v>
       </c>
       <c r="V7" s="16">
@@ -2695,14 +2723,14 @@
       <c r="H8" s="18">
         <v>26.989000000000001</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="23">
         <v>102891</v>
       </c>
       <c r="J8" s="16"/>
-      <c r="K8" s="31">
+      <c r="K8" s="23">
         <v>0.10100000000000001</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="23">
         <v>9.3350000000000009</v>
       </c>
       <c r="M8" s="16">
@@ -2717,14 +2745,14 @@
       <c r="Q8" s="18">
         <v>28.323</v>
       </c>
-      <c r="R8" s="31">
+      <c r="R8" s="23">
         <v>103228</v>
       </c>
       <c r="S8" s="16"/>
-      <c r="T8" s="31">
+      <c r="T8" s="23">
         <v>0.1</v>
       </c>
-      <c r="U8" s="31">
+      <c r="U8" s="23">
         <v>8.6059999999999999</v>
       </c>
       <c r="V8" s="16">
@@ -2756,14 +2784,14 @@
       <c r="H9" s="18">
         <v>24.521999999999998</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="23">
         <v>96521</v>
       </c>
       <c r="J9" s="16"/>
-      <c r="K9" s="31">
+      <c r="K9" s="23">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="23">
         <v>7.9829999999999997</v>
       </c>
       <c r="M9" s="16">
@@ -2778,14 +2806,14 @@
       <c r="Q9" s="18">
         <v>27.428000000000001</v>
       </c>
-      <c r="R9" s="31">
+      <c r="R9" s="23">
         <v>97173</v>
       </c>
       <c r="S9" s="16"/>
-      <c r="T9" s="31">
+      <c r="T9" s="23">
         <v>0.10199999999999999</v>
       </c>
-      <c r="U9" s="31">
+      <c r="U9" s="23">
         <v>10.391</v>
       </c>
       <c r="V9" s="16">
@@ -2817,14 +2845,14 @@
       <c r="H10" s="18">
         <v>22.553000000000001</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="23">
         <v>88323</v>
       </c>
       <c r="J10" s="16"/>
-      <c r="K10" s="31">
+      <c r="K10" s="23">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="L10" s="31">
+      <c r="L10" s="23">
         <v>7.9669999999999996</v>
       </c>
       <c r="M10" s="16">
@@ -2839,14 +2867,14 @@
       <c r="Q10" s="18">
         <v>25.245000000000001</v>
       </c>
-      <c r="R10" s="31">
+      <c r="R10" s="23">
         <v>88866</v>
       </c>
       <c r="S10" s="16"/>
-      <c r="T10" s="31">
+      <c r="T10" s="23">
         <v>0.10199999999999999</v>
       </c>
-      <c r="U10" s="31">
+      <c r="U10" s="23">
         <v>10.505000000000001</v>
       </c>
       <c r="V10" s="16">
@@ -2878,14 +2906,14 @@
       <c r="H11" s="18">
         <v>20.119</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I11" s="23">
         <v>80073</v>
       </c>
       <c r="J11" s="16"/>
-      <c r="K11" s="31">
+      <c r="K11" s="23">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="L11" s="31">
+      <c r="L11" s="23">
         <v>17.106999999999999</v>
       </c>
       <c r="M11" s="16">
@@ -2900,14 +2928,14 @@
       <c r="Q11" s="18">
         <v>22.638000000000002</v>
       </c>
-      <c r="R11" s="31">
+      <c r="R11" s="23">
         <v>78631</v>
       </c>
       <c r="S11" s="16"/>
-      <c r="T11" s="31">
+      <c r="T11" s="23">
         <v>0.11899999999999999</v>
       </c>
-      <c r="U11" s="31">
+      <c r="U11" s="23">
         <v>16.93</v>
       </c>
       <c r="V11" s="16">
@@ -2939,14 +2967,14 @@
       <c r="H12" s="18">
         <v>18.905000000000001</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="23">
         <v>79949</v>
       </c>
       <c r="J12" s="16"/>
-      <c r="K12" s="31">
+      <c r="K12" s="23">
         <v>9.4E-2</v>
       </c>
-      <c r="L12" s="31">
+      <c r="L12" s="23">
         <v>8.6319999999999997</v>
       </c>
       <c r="M12" s="16">
@@ -2961,14 +2989,14 @@
       <c r="Q12" s="18">
         <v>21.321000000000002</v>
       </c>
-      <c r="R12" s="31">
+      <c r="R12" s="23">
         <v>69870</v>
       </c>
       <c r="S12" s="16"/>
-      <c r="T12" s="31">
+      <c r="T12" s="23">
         <v>0.1</v>
       </c>
-      <c r="U12" s="31">
+      <c r="U12" s="23">
         <v>8.7430000000000003</v>
       </c>
       <c r="V12" s="16">
@@ -2981,26 +3009,26 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O15" s="23" t="s">
+      <c r="O15" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="27" t="s">
+      <c r="P15" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="Q15" s="21" t="s">
+      <c r="Q15" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="R15" s="22"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="21" t="s">
+      <c r="R15" s="27"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="U15" s="22"/>
-      <c r="V15" s="23"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="28"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O16" s="24"/>
-      <c r="P16" s="28"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="33"/>
       <c r="Q16" s="7" t="s">
         <v>12</v>
       </c>
@@ -3021,7 +3049,7 @@
       </c>
     </row>
     <row r="17" spans="15:22" x14ac:dyDescent="0.3">
-      <c r="O17" s="30">
+      <c r="O17" s="22">
         <v>0</v>
       </c>
       <c r="P17" s="17">
@@ -3054,14 +3082,14 @@
       <c r="Q18" s="18">
         <v>20.341000000000001</v>
       </c>
-      <c r="R18" s="31">
+      <c r="R18" s="23">
         <v>79949</v>
       </c>
       <c r="S18" s="16"/>
-      <c r="T18" s="31">
+      <c r="T18" s="23">
         <v>0.109</v>
       </c>
-      <c r="U18" s="31">
+      <c r="U18" s="23">
         <v>9.3439999999999994</v>
       </c>
       <c r="V18" s="16">
@@ -3078,14 +3106,14 @@
       <c r="Q19" s="18">
         <v>17.306999999999999</v>
       </c>
-      <c r="R19" s="31">
+      <c r="R19" s="23">
         <v>71312</v>
       </c>
       <c r="S19" s="16"/>
-      <c r="T19" s="31">
+      <c r="T19" s="23">
         <v>0.1</v>
       </c>
-      <c r="U19" s="31">
+      <c r="U19" s="23">
         <v>15.314</v>
       </c>
       <c r="V19" s="16">
@@ -3102,14 +3130,14 @@
       <c r="Q20" s="18">
         <v>17.437999999999999</v>
       </c>
-      <c r="R20" s="31">
+      <c r="R20" s="23">
         <v>69327</v>
       </c>
       <c r="S20" s="16"/>
-      <c r="T20" s="31">
+      <c r="T20" s="23">
         <v>0.09</v>
       </c>
-      <c r="U20" s="31">
+      <c r="U20" s="23">
         <v>11.083</v>
       </c>
       <c r="V20" s="16">
@@ -3126,14 +3154,14 @@
       <c r="Q21" s="18">
         <v>17.946999999999999</v>
       </c>
-      <c r="R21" s="31">
+      <c r="R21" s="23">
         <v>69218</v>
       </c>
       <c r="S21" s="16"/>
-      <c r="T21" s="31">
+      <c r="T21" s="23">
         <v>0.1</v>
       </c>
-      <c r="U21" s="31">
+      <c r="U21" s="23">
         <v>13.476000000000001</v>
       </c>
       <c r="V21" s="16">
@@ -3150,14 +3178,14 @@
       <c r="Q22" s="18">
         <v>18.53</v>
       </c>
-      <c r="R22" s="31">
+      <c r="R22" s="23">
         <v>69533</v>
       </c>
       <c r="S22" s="16"/>
-      <c r="T22" s="31">
+      <c r="T22" s="23">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="U22" s="31">
+      <c r="U22" s="23">
         <v>8.2609999999999992</v>
       </c>
       <c r="V22" s="16">
@@ -3174,14 +3202,14 @@
       <c r="Q23" s="18">
         <v>20.381</v>
       </c>
-      <c r="R23" s="31">
+      <c r="R23" s="23">
         <v>69870</v>
       </c>
       <c r="S23" s="16"/>
-      <c r="T23" s="31">
+      <c r="T23" s="23">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="U23" s="31">
+      <c r="U23" s="23">
         <v>14.048999999999999</v>
       </c>
       <c r="V23" s="16">

</xml_diff>

<commit_message>
Preparation for two additional tests
</commit_message>
<xml_diff>
--- a/input/core_algorithms_2022/Experiment_results.xlsx
+++ b/input/core_algorithms_2022/Experiment_results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_Devel\Repos\repos-2020-06\model-interplay-monitoring-code\input\core_algorithms_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1548674-ECC7-4459-A256-0703499919E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732ABDD0-2DA6-432B-8AD2-E7CE11B91AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3945" yWindow="-21720" windowWidth="38640" windowHeight="21390" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
   </bookViews>
   <sheets>
     <sheet name="modelSize" sheetId="6" r:id="rId1"/>
     <sheet name="conditions" sheetId="7" r:id="rId2"/>
     <sheet name="syncPoints" sheetId="8" r:id="rId3"/>
+    <sheet name="modelCount" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="92">
   <si>
     <t>States</t>
   </si>
@@ -56,18 +57,6 @@
     <t>Event Processing Time (ms)</t>
   </si>
   <si>
-    <t>Model size without data</t>
-  </si>
-  <si>
-    <t>Model size with data</t>
-  </si>
-  <si>
-    <t>Syncronisation activity placement in control flow</t>
-  </si>
-  <si>
-    <t>Number of syncronisation activities (beginning -&gt; end)</t>
-  </si>
-  <si>
     <t>Mean</t>
   </si>
   <si>
@@ -104,12 +93,6 @@
     <t>Constraints after</t>
   </si>
   <si>
-    <t>Guard placement in control flow</t>
-  </si>
-  <si>
-    <t>Number of guards (beginning -&gt; end)</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -281,9 +264,6 @@
     <t>12/24</t>
   </si>
   <si>
-    <t>Number of guards (end -&gt; beginning)</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -294,6 +274,45 @@
   </si>
   <si>
     <t>NB! The non-deterministic nature of Java GC means that memory consumption with the same inputs may vary significantly (up to multiple GB in some tests), values given here should be seen as indicative of the overal trend only.</t>
+  </si>
+  <si>
+    <t>01 Model size without data</t>
+  </si>
+  <si>
+    <t>02 Model size with data</t>
+  </si>
+  <si>
+    <t>03 Guard placement in control flow</t>
+  </si>
+  <si>
+    <t>04 Number of guards (beginning -&gt; end)</t>
+  </si>
+  <si>
+    <t>05 Number of guards (end -&gt; beginning)</t>
+  </si>
+  <si>
+    <t>06 Syncronisation activity placement in control flow</t>
+  </si>
+  <si>
+    <t>07 Number of syncronisation activities (beginning -&gt; end)</t>
+  </si>
+  <si>
+    <t>08 Number of syncronisation activities (beginning -&gt; end)</t>
+  </si>
+  <si>
+    <t>Specifications</t>
+  </si>
+  <si>
+    <t>DPN</t>
+  </si>
+  <si>
+    <t>LMP-Declare</t>
+  </si>
+  <si>
+    <t>09 Number of input models without data</t>
+  </si>
+  <si>
+    <t>10 Number of input models with data</t>
   </si>
 </sst>
 </file>
@@ -446,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -511,6 +530,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -534,6 +562,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,7 +895,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E4" sqref="E4:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -864,53 +907,53 @@
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="32"/>
+      <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="D5" s="36"/>
       <c r="E5" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>2</v>
@@ -919,7 +962,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -927,10 +970,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D6" s="14">
         <v>1</v>
@@ -959,10 +1002,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="D7" s="14">
         <v>2</v>
@@ -991,10 +1034,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="D8" s="14">
         <v>3</v>
@@ -1023,10 +1066,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="D9" s="14">
         <v>4</v>
@@ -1055,10 +1098,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="D10" s="14">
         <v>5</v>
@@ -1087,10 +1130,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="D11" s="14">
         <v>6</v>
@@ -1119,10 +1162,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="D12" s="14">
         <v>7</v>
@@ -1148,58 +1191,58 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="31"/>
+      <c r="F15" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="30"/>
+      <c r="L15" s="31"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="32"/>
+      <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="26" t="s">
+      <c r="C16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" s="27"/>
-      <c r="L15" s="28"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
-      <c r="B16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D16" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="F16" s="36"/>
       <c r="G16" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>2</v>
@@ -1208,7 +1251,7 @@
         <v>3</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1216,16 +1259,16 @@
         <v>0</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F17" s="14">
         <v>1</v>
@@ -1254,16 +1297,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="D18" s="13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F18" s="14">
         <v>2</v>
@@ -1292,16 +1335,16 @@
         <v>2</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="D19" s="13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F19" s="14">
         <v>3</v>
@@ -1330,16 +1373,16 @@
         <v>3</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="D20" s="13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F20" s="14">
         <v>4</v>
@@ -1368,16 +1411,16 @@
         <v>4</v>
       </c>
       <c r="B21" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="D21" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F21" s="14">
         <v>5</v>
@@ -1406,16 +1449,16 @@
         <v>5</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>53</v>
-      </c>
       <c r="D22" s="13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F22" s="14">
         <v>6</v>
@@ -1444,16 +1487,16 @@
         <v>6</v>
       </c>
       <c r="B23" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>54</v>
-      </c>
       <c r="D23" s="13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F23" s="14">
         <v>7</v>
@@ -1505,7 +1548,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1520,87 +1563,87 @@
   <sheetData>
     <row r="1" spans="1:24" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="26" t="s">
+      <c r="B4" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="31"/>
+      <c r="F4" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="26" t="s">
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
-      <c r="O4" s="28" t="s">
+      <c r="L4" s="30"/>
+      <c r="M4" s="31"/>
+      <c r="O4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" s="30"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="V4" s="30"/>
+      <c r="W4" s="31"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="32"/>
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="S4" s="27"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="V4" s="27"/>
-      <c r="W4" s="28"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>2</v>
@@ -1609,23 +1652,23 @@
         <v>3</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O5" s="29"/>
+        <v>6</v>
+      </c>
+      <c r="O5" s="32"/>
       <c r="P5" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="S5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="U5" s="7" t="s">
         <v>2</v>
@@ -1634,7 +1677,7 @@
         <v>3</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -1642,22 +1685,22 @@
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H6" s="18">
         <v>28.274000000000001</v>
@@ -1679,10 +1722,10 @@
         <v>0</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="R6" s="18">
         <v>28.257999999999999</v>
@@ -1706,19 +1749,19 @@
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G7" s="14">
         <v>6</v>
@@ -1743,10 +1786,10 @@
         <v>1</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="R7" s="18">
         <v>35.768999999999998</v>
@@ -1770,19 +1813,19 @@
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G8" s="14">
         <v>5</v>
@@ -1807,10 +1850,10 @@
         <v>2</v>
       </c>
       <c r="P8" s="13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="R8" s="18">
         <v>47.673000000000002</v>
@@ -1834,19 +1877,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G9" s="14">
         <v>4</v>
@@ -1871,10 +1914,10 @@
         <v>3</v>
       </c>
       <c r="P9" s="13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R9" s="18">
         <v>56.835000000000001</v>
@@ -1898,19 +1941,19 @@
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G10" s="14">
         <v>3</v>
@@ -1935,10 +1978,10 @@
         <v>4</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="R10" s="18">
         <v>73.058000000000007</v>
@@ -1962,19 +2005,19 @@
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G11" s="14">
         <v>2</v>
@@ -1999,10 +2042,10 @@
         <v>5</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="R11" s="18">
         <v>98.23</v>
@@ -2026,19 +2069,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G12" s="14">
         <v>1</v>
@@ -2063,10 +2106,10 @@
         <v>6</v>
       </c>
       <c r="P12" s="13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="R12" s="18">
         <v>136.50299999999999</v>
@@ -2090,19 +2133,19 @@
         <v>7</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G13" s="14">
         <v>0</v>
@@ -2127,10 +2170,10 @@
         <v>7</v>
       </c>
       <c r="P13" s="20" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="Q13" s="11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="R13" s="18">
         <v>212.702</v>
@@ -2152,44 +2195,44 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O15" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="O16" s="28" t="s">
+      <c r="O16" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="P16" s="26" t="s">
+      <c r="P16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="S16" s="30"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="V16" s="30"/>
+      <c r="W16" s="31"/>
+    </row>
+    <row r="17" spans="15:24" x14ac:dyDescent="0.3">
+      <c r="O17" s="32"/>
+      <c r="P17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="S16" s="27"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="V16" s="27"/>
-      <c r="W16" s="28"/>
-    </row>
-    <row r="17" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O17" s="29"/>
-      <c r="P17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q17" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="R17" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="S17" s="7" t="s">
         <v>0</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="U17" s="7" t="s">
         <v>2</v>
@@ -2198,7 +2241,7 @@
         <v>3</v>
       </c>
       <c r="W17" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="15:24" x14ac:dyDescent="0.3">
@@ -2206,10 +2249,10 @@
         <v>0</v>
       </c>
       <c r="P18" s="18" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="Q18" s="16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="R18" s="18">
         <v>27.352</v>
@@ -2233,10 +2276,10 @@
         <v>1</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="Q19" s="11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="R19" s="18">
         <v>44.231999999999999</v>
@@ -2260,10 +2303,10 @@
         <v>2</v>
       </c>
       <c r="P20" s="13" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="Q20" s="11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="R20" s="18">
         <v>67.411000000000001</v>
@@ -2287,10 +2330,10 @@
         <v>3</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="Q21" s="11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R21" s="18">
         <v>87.522999999999996</v>
@@ -2314,10 +2357,10 @@
         <v>4</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="Q22" s="11" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="R22" s="18">
         <v>116.637</v>
@@ -2341,10 +2384,10 @@
         <v>5</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="Q23" s="11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="R23" s="18">
         <v>149.12</v>
@@ -2368,10 +2411,10 @@
         <v>6</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="Q24" s="11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="R24" s="18">
         <v>182.76400000000001</v>
@@ -2395,10 +2438,10 @@
         <v>7</v>
       </c>
       <c r="P25" s="20" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="Q25" s="11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="R25" s="18">
         <v>224.78</v>
@@ -2420,13 +2463,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:J4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="P16:Q16"/>
@@ -2435,6 +2471,13 @@
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="U16:W16"/>
     <mergeCell ref="O16:O17"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2451,7 +2494,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2465,86 +2508,86 @@
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="31"/>
+      <c r="F4" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="30"/>
+      <c r="M4" s="31"/>
+      <c r="O4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="30"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" s="30"/>
+      <c r="V4" s="31"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="32"/>
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
-      <c r="O4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P4" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q4" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="R4" s="27"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="U4" s="27"/>
-      <c r="V4" s="28"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>2</v>
@@ -2553,18 +2596,18 @@
         <v>3</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O5" s="29"/>
-      <c r="P5" s="33"/>
+        <v>6</v>
+      </c>
+      <c r="O5" s="32"/>
+      <c r="P5" s="36"/>
       <c r="Q5" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="R5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="T5" s="7" t="s">
         <v>2</v>
@@ -2573,7 +2616,7 @@
         <v>3</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
@@ -2581,22 +2624,22 @@
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H6" s="18">
         <v>27.649000000000001</v>
@@ -2642,19 +2685,19 @@
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>53</v>
-      </c>
       <c r="F7" s="11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G7" s="14">
         <v>6</v>
@@ -2703,19 +2746,19 @@
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="D8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="F8" s="11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G8" s="14">
         <v>5</v>
@@ -2764,19 +2807,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="D9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="F9" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G9" s="14">
         <v>4</v>
@@ -2825,19 +2868,19 @@
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="D10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="F10" s="11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G10" s="14">
         <v>3</v>
@@ -2886,19 +2929,19 @@
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>52</v>
-      </c>
       <c r="D11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="F11" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G11" s="14">
         <v>2</v>
@@ -2947,19 +2990,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>53</v>
-      </c>
       <c r="D12" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G12" s="14">
         <v>1</v>
@@ -3005,38 +3048,38 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="O14" s="2" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O15" s="28" t="s">
+      <c r="O15" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q15" s="26" t="s">
+      <c r="P15" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q15" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="R15" s="27"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="26" t="s">
+      <c r="R15" s="30"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="U15" s="27"/>
-      <c r="V15" s="28"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="31"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O16" s="29"/>
-      <c r="P16" s="33"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="36"/>
       <c r="Q16" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="R16" s="7" t="s">
         <v>0</v>
       </c>
       <c r="S16" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="T16" s="7" t="s">
         <v>2</v>
@@ -3045,7 +3088,7 @@
         <v>3</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="15:22" x14ac:dyDescent="0.3">
@@ -3240,4 +3283,344 @@
     <ignoredError sqref="F7 F8:F12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3842E7B5-15B7-4425-8C64-F08166DDE0AC}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="11.296875" customWidth="1"/>
+    <col min="4" max="6" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="30"/>
+      <c r="I4" s="31"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="32"/>
+      <c r="B5" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
+        <v>0</v>
+      </c>
+      <c r="B6" s="37">
+        <v>1</v>
+      </c>
+      <c r="C6" s="38">
+        <v>0</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="37">
+        <v>2</v>
+      </c>
+      <c r="C7" s="38">
+        <v>1</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="27"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="37">
+        <v>3</v>
+      </c>
+      <c r="C8" s="38">
+        <v>2</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="37">
+        <v>4</v>
+      </c>
+      <c r="C9" s="38">
+        <v>3</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>4</v>
+      </c>
+      <c r="B10" s="37">
+        <v>5</v>
+      </c>
+      <c r="C10" s="38">
+        <v>4</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>5</v>
+      </c>
+      <c r="B11" s="37">
+        <v>6</v>
+      </c>
+      <c r="C11" s="38">
+        <v>5</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="32"/>
+      <c r="B15" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="15">
+        <v>0</v>
+      </c>
+      <c r="B16" s="37">
+        <v>1</v>
+      </c>
+      <c r="C16" s="38">
+        <v>0</v>
+      </c>
+      <c r="D16" s="26"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="27"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="37">
+        <v>2</v>
+      </c>
+      <c r="C17" s="38">
+        <v>1</v>
+      </c>
+      <c r="D17" s="26"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="27"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>2</v>
+      </c>
+      <c r="B18" s="37">
+        <v>3</v>
+      </c>
+      <c r="C18" s="38">
+        <v>2</v>
+      </c>
+      <c r="D18" s="26"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>3</v>
+      </c>
+      <c r="B19" s="37">
+        <v>4</v>
+      </c>
+      <c r="C19" s="38">
+        <v>3</v>
+      </c>
+      <c r="D19" s="26"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="27"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>4</v>
+      </c>
+      <c r="B20" s="37">
+        <v>5</v>
+      </c>
+      <c r="C20" s="38">
+        <v>4</v>
+      </c>
+      <c r="D20" s="26"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="27"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>5</v>
+      </c>
+      <c r="B21" s="37">
+        <v>6</v>
+      </c>
+      <c r="C21" s="38">
+        <v>5</v>
+      </c>
+      <c r="D21" s="26"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Switched last two test from PU DPN to VT DPN
</commit_message>
<xml_diff>
--- a/input/core_algorithms_2022/Experiment_results.xlsx
+++ b/input/core_algorithms_2022/Experiment_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_Devel\Repos\repos-2020-06\model-interplay-monitoring-code\input\core_algorithms_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732ABDD0-2DA6-432B-8AD2-E7CE11B91AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2C6436-1440-4ABD-9A84-2B2792B878F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
+    <workbookView xWindow="-4350" yWindow="-12150" windowWidth="21600" windowHeight="11505" activeTab="3" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
   </bookViews>
   <sheets>
     <sheet name="modelSize" sheetId="6" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -539,6 +539,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -563,21 +584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -894,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D70222-B554-4BB9-8CB5-22FD4E14CBB3}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:J12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -916,36 +923,36 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="35" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="29" t="s">
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="31"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="43"/>
       <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1195,33 +1202,33 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="29" t="s">
+      <c r="C15" s="38"/>
+      <c r="D15" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="35" t="s">
+      <c r="E15" s="38"/>
+      <c r="F15" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="29" t="s">
+      <c r="H15" s="37"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="30"/>
-      <c r="L15" s="31"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="38"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
@@ -1234,7 +1241,7 @@
       <c r="E16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="36"/>
+      <c r="F16" s="43"/>
       <c r="G16" s="7" t="s">
         <v>8</v>
       </c>
@@ -1575,53 +1582,53 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="29" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="35" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="29" t="s">
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="30"/>
-      <c r="M4" s="31"/>
-      <c r="O4" s="31" t="s">
+      <c r="L4" s="37"/>
+      <c r="M4" s="38"/>
+      <c r="O4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="29" t="s">
+      <c r="P4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="29" t="s">
+      <c r="Q4" s="38"/>
+      <c r="R4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="30"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="29" t="s">
+      <c r="S4" s="37"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="30"/>
-      <c r="W4" s="31"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="38"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
@@ -1634,8 +1641,8 @@
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1654,7 +1661,7 @@
       <c r="M5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="32"/>
+      <c r="O5" s="39"/>
       <c r="P5" s="7" t="s">
         <v>14</v>
       </c>
@@ -2199,26 +2206,26 @@
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="O16" s="31" t="s">
+      <c r="O16" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="P16" s="29" t="s">
+      <c r="P16" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="29" t="s">
+      <c r="Q16" s="38"/>
+      <c r="R16" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="S16" s="30"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="29" t="s">
+      <c r="S16" s="37"/>
+      <c r="T16" s="38"/>
+      <c r="U16" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="V16" s="30"/>
-      <c r="W16" s="31"/>
+      <c r="V16" s="37"/>
+      <c r="W16" s="38"/>
     </row>
     <row r="17" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O17" s="32"/>
+      <c r="O17" s="39"/>
       <c r="P17" s="7" t="s">
         <v>14</v>
       </c>
@@ -2463,6 +2470,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="P16:Q16"/>
@@ -2471,13 +2485,6 @@
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="U16:W16"/>
     <mergeCell ref="O16:O17"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2520,52 +2527,52 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="29" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="35" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="29" t="s">
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="30"/>
-      <c r="M4" s="31"/>
-      <c r="O4" s="31" t="s">
+      <c r="L4" s="37"/>
+      <c r="M4" s="38"/>
+      <c r="O4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="35" t="s">
+      <c r="P4" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="29" t="s">
+      <c r="Q4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="30"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="29" t="s">
+      <c r="R4" s="37"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="30"/>
-      <c r="V4" s="31"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="38"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
@@ -2578,8 +2585,8 @@
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
@@ -2598,8 +2605,8 @@
       <c r="M5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="32"/>
-      <c r="P5" s="36"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="43"/>
       <c r="Q5" s="7" t="s">
         <v>8</v>
       </c>
@@ -3052,26 +3059,26 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O15" s="31" t="s">
+      <c r="O15" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="35" t="s">
+      <c r="P15" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="Q15" s="29" t="s">
+      <c r="Q15" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="R15" s="30"/>
-      <c r="S15" s="31"/>
-      <c r="T15" s="29" t="s">
+      <c r="R15" s="37"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="U15" s="30"/>
-      <c r="V15" s="31"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="38"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O16" s="32"/>
-      <c r="P16" s="36"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="43"/>
       <c r="Q16" s="7" t="s">
         <v>8</v>
       </c>
@@ -3287,10 +3294,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3842E7B5-15B7-4425-8C64-F08166DDE0AC}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3299,41 +3306,41 @@
     <col min="4" max="6" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="29" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="29" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="39" t="s">
+      <c r="H4" s="37"/>
+      <c r="I4" s="38"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="34" t="s">
         <v>89</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -3355,48 +3362,49 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>0</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="31">
         <v>1</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="32">
         <v>0</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="23"/>
-      <c r="F6" s="41"/>
+      <c r="F6" s="35"/>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
-      <c r="I6" s="27"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I6" s="30"/>
+      <c r="K6" s="44"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B7" s="31">
         <v>2</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="32">
         <v>1</v>
       </c>
-      <c r="D7" s="26"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="23"/>
-      <c r="F7" s="27"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
-      <c r="I7" s="27"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I7" s="30"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="31">
         <v>3</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="32">
         <v>2</v>
       </c>
       <c r="D8" s="26"/>
@@ -3406,14 +3414,14 @@
       <c r="H8" s="23"/>
       <c r="I8" s="27"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="31">
         <v>4</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="32">
         <v>3</v>
       </c>
       <c r="D9" s="26"/>
@@ -3423,14 +3431,14 @@
       <c r="H9" s="23"/>
       <c r="I9" s="27"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>4</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="31">
         <v>5</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="32">
         <v>4</v>
       </c>
       <c r="D10" s="26"/>
@@ -3440,14 +3448,14 @@
       <c r="H10" s="23"/>
       <c r="I10" s="27"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B11" s="37">
+      <c r="B11" s="31">
         <v>6</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="32">
         <v>5</v>
       </c>
       <c r="D11" s="26"/>
@@ -3457,36 +3465,36 @@
       <c r="H11" s="23"/>
       <c r="I11" s="27"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="29" t="s">
+      <c r="C14" s="41"/>
+      <c r="D14" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="29" t="s">
+      <c r="E14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="31"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="39" t="s">
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="39"/>
+      <c r="B15" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="34" t="s">
         <v>89</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -3508,19 +3516,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>0</v>
       </c>
-      <c r="B16" s="37">
+      <c r="B16" s="31">
         <v>1</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="32">
         <v>0</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="41"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
       <c r="I16" s="27"/>
@@ -3529,10 +3537,10 @@
       <c r="A17" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="37">
+      <c r="B17" s="31">
         <v>2</v>
       </c>
-      <c r="C17" s="38">
+      <c r="C17" s="32">
         <v>1</v>
       </c>
       <c r="D17" s="26"/>
@@ -3546,10 +3554,10 @@
       <c r="A18" s="1">
         <v>2</v>
       </c>
-      <c r="B18" s="37">
+      <c r="B18" s="31">
         <v>3</v>
       </c>
-      <c r="C18" s="38">
+      <c r="C18" s="32">
         <v>2</v>
       </c>
       <c r="D18" s="26"/>
@@ -3563,10 +3571,10 @@
       <c r="A19" s="1">
         <v>3</v>
       </c>
-      <c r="B19" s="37">
+      <c r="B19" s="31">
         <v>4</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="32">
         <v>3</v>
       </c>
       <c r="D19" s="26"/>
@@ -3580,10 +3588,10 @@
       <c r="A20" s="1">
         <v>4</v>
       </c>
-      <c r="B20" s="37">
+      <c r="B20" s="31">
         <v>5</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="32">
         <v>4</v>
       </c>
       <c r="D20" s="26"/>
@@ -3597,10 +3605,10 @@
       <c r="A21" s="1">
         <v>5</v>
       </c>
-      <c r="B21" s="37">
+      <c r="B21" s="31">
         <v>6</v>
       </c>
-      <c r="C21" s="38">
+      <c r="C21" s="32">
         <v>5</v>
       </c>
       <c r="D21" s="26"/>

</xml_diff>

<commit_message>
Eventlog for the final two sets of tests
</commit_message>
<xml_diff>
--- a/input/core_algorithms_2022/Experiment_results.xlsx
+++ b/input/core_algorithms_2022/Experiment_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_Devel\Repos\repos-2020-06\model-interplay-monitoring-code\input\core_algorithms_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2C6436-1440-4ABD-9A84-2B2792B878F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5705C8-3663-4A22-9B6F-5BE39C942DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4350" yWindow="-12150" windowWidth="21600" windowHeight="11505" activeTab="3" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
   </bookViews>
   <sheets>
     <sheet name="modelSize" sheetId="6" r:id="rId1"/>
@@ -560,6 +560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -584,7 +585,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,36 +923,36 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="36" t="s">
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="37"/>
-      <c r="J4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="44"/>
       <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1202,33 +1202,33 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="36" t="s">
+      <c r="C15" s="39"/>
+      <c r="D15" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="42" t="s">
+      <c r="E15" s="39"/>
+      <c r="F15" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="36" t="s">
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="37"/>
-      <c r="L15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="39"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
@@ -1241,7 +1241,7 @@
       <c r="E16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="43"/>
+      <c r="F16" s="44"/>
       <c r="G16" s="7" t="s">
         <v>8</v>
       </c>
@@ -1582,53 +1582,53 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="36" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="42" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="37"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="36" t="s">
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="37"/>
-      <c r="M4" s="38"/>
-      <c r="O4" s="38" t="s">
+      <c r="L4" s="38"/>
+      <c r="M4" s="39"/>
+      <c r="O4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="36" t="s">
+      <c r="P4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="36" t="s">
+      <c r="Q4" s="39"/>
+      <c r="R4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="37"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="36" t="s">
+      <c r="S4" s="38"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="37"/>
-      <c r="W4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="39"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
@@ -1641,8 +1641,8 @@
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1661,7 +1661,7 @@
       <c r="M5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="39"/>
+      <c r="O5" s="40"/>
       <c r="P5" s="7" t="s">
         <v>14</v>
       </c>
@@ -2206,26 +2206,26 @@
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="O16" s="38" t="s">
+      <c r="O16" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="P16" s="36" t="s">
+      <c r="P16" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="36" t="s">
+      <c r="Q16" s="39"/>
+      <c r="R16" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="S16" s="37"/>
-      <c r="T16" s="38"/>
-      <c r="U16" s="36" t="s">
+      <c r="S16" s="38"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="V16" s="37"/>
-      <c r="W16" s="38"/>
+      <c r="V16" s="38"/>
+      <c r="W16" s="39"/>
     </row>
     <row r="17" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O17" s="39"/>
+      <c r="O17" s="40"/>
       <c r="P17" s="7" t="s">
         <v>14</v>
       </c>
@@ -2470,13 +2470,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:J4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="P16:Q16"/>
@@ -2485,6 +2478,13 @@
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="U16:W16"/>
     <mergeCell ref="O16:O17"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2527,52 +2527,52 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="36" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="42" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="37"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="36" t="s">
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="37"/>
-      <c r="M4" s="38"/>
-      <c r="O4" s="38" t="s">
+      <c r="L4" s="38"/>
+      <c r="M4" s="39"/>
+      <c r="O4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="42" t="s">
+      <c r="P4" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="36" t="s">
+      <c r="Q4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="37"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="36" t="s">
+      <c r="R4" s="38"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="37"/>
-      <c r="V4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="39"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
@@ -2585,8 +2585,8 @@
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
@@ -2605,8 +2605,8 @@
       <c r="M5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="39"/>
-      <c r="P5" s="43"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="44"/>
       <c r="Q5" s="7" t="s">
         <v>8</v>
       </c>
@@ -3059,26 +3059,26 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O15" s="38" t="s">
+      <c r="O15" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="42" t="s">
+      <c r="P15" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="Q15" s="36" t="s">
+      <c r="Q15" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="R15" s="37"/>
-      <c r="S15" s="38"/>
-      <c r="T15" s="36" t="s">
+      <c r="R15" s="38"/>
+      <c r="S15" s="39"/>
+      <c r="T15" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="U15" s="37"/>
-      <c r="V15" s="38"/>
+      <c r="U15" s="38"/>
+      <c r="V15" s="39"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O16" s="39"/>
-      <c r="P16" s="43"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="44"/>
       <c r="Q16" s="7" t="s">
         <v>8</v>
       </c>
@@ -3296,8 +3296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3842E7B5-15B7-4425-8C64-F08166DDE0AC}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3317,26 +3317,26 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="36" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="36" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="33" t="s">
         <v>88</v>
       </c>
@@ -3378,7 +3378,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
       <c r="I6" s="30"/>
-      <c r="K6" s="44"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -3471,26 +3471,26 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="36" t="s">
+      <c r="C14" s="42"/>
+      <c r="D14" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="36" t="s">
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="37"/>
-      <c r="I14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="33" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Final two sets of tests done
</commit_message>
<xml_diff>
--- a/input/core_algorithms_2022/Experiment_results.xlsx
+++ b/input/core_algorithms_2022/Experiment_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_Devel\Repos\repos-2020-06\model-interplay-monitoring-code\input\core_algorithms_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5705C8-3663-4A22-9B6F-5BE39C942DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1EB6F3-6D3C-4AB3-B216-2B6640C1C4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
+    <workbookView xWindow="-3945" yWindow="-21720" windowWidth="38640" windowHeight="21390" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
   </bookViews>
   <sheets>
     <sheet name="modelSize" sheetId="6" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -530,19 +530,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -561,6 +549,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -901,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D70222-B554-4BB9-8CB5-22FD4E14CBB3}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -923,36 +917,36 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="37" t="s">
+      <c r="F4" s="36"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="37"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1202,33 +1196,33 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="37" t="s">
+      <c r="C15" s="37"/>
+      <c r="D15" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="43" t="s">
+      <c r="E15" s="37"/>
+      <c r="F15" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="37" t="s">
+      <c r="H15" s="36"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="38"/>
-      <c r="L15" s="39"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="37"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="40"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
@@ -1241,7 +1235,7 @@
       <c r="E16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="44"/>
+      <c r="F16" s="42"/>
       <c r="G16" s="7" t="s">
         <v>8</v>
       </c>
@@ -1555,7 +1549,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1582,53 +1576,53 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="37" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="43" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="37" t="s">
+      <c r="I4" s="36"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="38"/>
-      <c r="M4" s="39"/>
-      <c r="O4" s="39" t="s">
+      <c r="L4" s="36"/>
+      <c r="M4" s="37"/>
+      <c r="O4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="37" t="s">
+      <c r="P4" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="37" t="s">
+      <c r="Q4" s="37"/>
+      <c r="R4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="38"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="37" t="s">
+      <c r="S4" s="36"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="38"/>
-      <c r="W4" s="39"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="37"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
@@ -1641,8 +1635,8 @@
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1661,7 +1655,7 @@
       <c r="M5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="40"/>
+      <c r="O5" s="38"/>
       <c r="P5" s="7" t="s">
         <v>14</v>
       </c>
@@ -2206,26 +2200,26 @@
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="O16" s="39" t="s">
+      <c r="O16" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="P16" s="37" t="s">
+      <c r="P16" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="37" t="s">
+      <c r="Q16" s="37"/>
+      <c r="R16" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="S16" s="38"/>
-      <c r="T16" s="39"/>
-      <c r="U16" s="37" t="s">
+      <c r="S16" s="36"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="V16" s="38"/>
-      <c r="W16" s="39"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="37"/>
     </row>
     <row r="17" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O17" s="40"/>
+      <c r="O17" s="38"/>
       <c r="P17" s="7" t="s">
         <v>14</v>
       </c>
@@ -2470,6 +2464,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="P16:Q16"/>
@@ -2478,13 +2479,6 @@
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="U16:W16"/>
     <mergeCell ref="O16:O17"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2501,7 +2495,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2527,52 +2521,52 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="37" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="43" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="37" t="s">
+      <c r="I4" s="36"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="38"/>
-      <c r="M4" s="39"/>
-      <c r="O4" s="39" t="s">
+      <c r="L4" s="36"/>
+      <c r="M4" s="37"/>
+      <c r="O4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="43" t="s">
+      <c r="P4" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="38"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="37" t="s">
+      <c r="R4" s="36"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="38"/>
-      <c r="V4" s="39"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="37"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
@@ -2585,8 +2579,8 @@
       <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="7" t="s">
         <v>8</v>
       </c>
@@ -2605,8 +2599,8 @@
       <c r="M5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="40"/>
-      <c r="P5" s="44"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="42"/>
       <c r="Q5" s="7" t="s">
         <v>8</v>
       </c>
@@ -3059,26 +3053,26 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O15" s="39" t="s">
+      <c r="O15" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="43" t="s">
+      <c r="P15" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="Q15" s="37" t="s">
+      <c r="Q15" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="R15" s="38"/>
-      <c r="S15" s="39"/>
-      <c r="T15" s="37" t="s">
+      <c r="R15" s="36"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="U15" s="38"/>
-      <c r="V15" s="39"/>
+      <c r="U15" s="36"/>
+      <c r="V15" s="37"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O16" s="40"/>
-      <c r="P16" s="44"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="42"/>
       <c r="Q16" s="7" t="s">
         <v>8</v>
       </c>
@@ -3296,8 +3290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3842E7B5-15B7-4425-8C64-F08166DDE0AC}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3317,30 +3311,30 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="37" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="37" t="s">
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="37"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="33" t="s">
+      <c r="A5" s="38"/>
+      <c r="B5" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>89</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -3349,7 +3343,7 @@
       <c r="E5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="26" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -3358,7 +3352,7 @@
       <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="26" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3366,104 +3360,176 @@
       <c r="A6" s="15">
         <v>0</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="27">
         <v>1</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="28">
         <v>0</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="30"/>
-      <c r="K6" s="36"/>
+      <c r="D6" s="33">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E6" s="23">
+        <v>4</v>
+      </c>
+      <c r="F6" s="31">
+        <v>174</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="H6" s="23">
+        <v>24.12</v>
+      </c>
+      <c r="I6" s="34">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="27">
         <v>2</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="28">
         <v>1</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="30"/>
+      <c r="D7" s="33">
+        <v>2.3E-2</v>
+      </c>
+      <c r="E7" s="23">
+        <v>36</v>
+      </c>
+      <c r="F7" s="34">
+        <v>175</v>
+      </c>
+      <c r="G7" s="23">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="H7" s="23">
+        <v>22.478999999999999</v>
+      </c>
+      <c r="I7" s="34">
+        <v>0.34200000000000003</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="27">
         <v>3</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="28">
         <v>2</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="27"/>
+      <c r="D8" s="33">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E8" s="23">
+        <v>216</v>
+      </c>
+      <c r="F8" s="34">
+        <v>179</v>
+      </c>
+      <c r="G8" s="23">
+        <v>0.105</v>
+      </c>
+      <c r="H8" s="23">
+        <v>20.117000000000001</v>
+      </c>
+      <c r="I8" s="34">
+        <v>0.378</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="27">
         <v>4</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="28">
         <v>3</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="27"/>
+      <c r="D9" s="33">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="E9" s="23">
+        <v>1296</v>
+      </c>
+      <c r="F9" s="34">
+        <v>185</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="H9" s="23">
+        <v>26.167999999999999</v>
+      </c>
+      <c r="I9" s="34">
+        <v>0.41499999999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>4</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="27">
         <v>5</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="28">
         <v>4</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="27"/>
+      <c r="D10" s="33">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="E10" s="23">
+        <v>7776</v>
+      </c>
+      <c r="F10" s="34">
+        <v>242</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="H10" s="23">
+        <v>33.045000000000002</v>
+      </c>
+      <c r="I10" s="34">
+        <v>0.441</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="27">
         <v>6</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="28">
         <v>5</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="27"/>
+      <c r="D11" s="33">
+        <v>2.7010000000000001</v>
+      </c>
+      <c r="E11" s="23">
+        <v>46656</v>
+      </c>
+      <c r="F11" s="34">
+        <v>702</v>
+      </c>
+      <c r="G11" s="23">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="H11" s="23">
+        <v>28.323</v>
+      </c>
+      <c r="I11" s="34">
+        <v>0.48799999999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -3471,30 +3537,30 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="37" t="s">
+      <c r="C14" s="40"/>
+      <c r="D14" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="37" t="s">
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="37"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="33" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="30" t="s">
         <v>89</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -3503,7 +3569,7 @@
       <c r="E15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="26" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="7" t="s">
@@ -3512,7 +3578,7 @@
       <c r="H15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="26" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3520,103 +3586,175 @@
       <c r="A16" s="15">
         <v>0</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="27">
         <v>1</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="28">
         <v>0</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="27"/>
+      <c r="D16" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="E16" s="23">
+        <v>6</v>
+      </c>
+      <c r="F16" s="31">
+        <v>178</v>
+      </c>
+      <c r="G16" s="23">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="H16" s="23">
+        <v>16.481000000000002</v>
+      </c>
+      <c r="I16" s="34">
+        <v>0.311</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="27">
         <v>2</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="28">
         <v>1</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="27"/>
+      <c r="D17" s="33">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="E17" s="23">
+        <v>64</v>
+      </c>
+      <c r="F17" s="34">
+        <v>179</v>
+      </c>
+      <c r="G17" s="23">
+        <v>0.104</v>
+      </c>
+      <c r="H17" s="23">
+        <v>18.888999999999999</v>
+      </c>
+      <c r="I17" s="34">
+        <v>0.38700000000000001</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="27">
         <v>3</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="28">
         <v>2</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="27"/>
+      <c r="D18" s="33">
+        <v>0.111</v>
+      </c>
+      <c r="E18" s="23">
+        <v>512</v>
+      </c>
+      <c r="F18" s="34">
+        <v>187</v>
+      </c>
+      <c r="G18" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="H18" s="23">
+        <v>18.042999999999999</v>
+      </c>
+      <c r="I18" s="34">
+        <v>0.45900000000000002</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>3</v>
       </c>
-      <c r="B19" s="31">
+      <c r="B19" s="27">
         <v>4</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="28">
         <v>3</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="27"/>
+      <c r="D19" s="33">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="E19" s="23">
+        <v>4096</v>
+      </c>
+      <c r="F19" s="34">
+        <v>276</v>
+      </c>
+      <c r="G19" s="23">
+        <v>0.115</v>
+      </c>
+      <c r="H19" s="23">
+        <v>22.178000000000001</v>
+      </c>
+      <c r="I19" s="34">
+        <v>0.50800000000000001</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>4</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="27">
         <v>5</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="28">
         <v>4</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="27"/>
+      <c r="D20" s="33">
+        <v>5.1369999999999996</v>
+      </c>
+      <c r="E20" s="23">
+        <v>32768</v>
+      </c>
+      <c r="F20" s="34">
+        <v>1174</v>
+      </c>
+      <c r="G20" s="23">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H20" s="23">
+        <v>10.35</v>
+      </c>
+      <c r="I20" s="34">
+        <v>0.438</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>5</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="27">
         <v>6</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="28">
         <v>5</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="27"/>
+      <c r="D21" s="33">
+        <v>54.033999999999999</v>
+      </c>
+      <c r="E21" s="23">
+        <v>262144</v>
+      </c>
+      <c r="F21" s="34">
+        <v>9013</v>
+      </c>
+      <c r="G21" s="23">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H21" s="23">
+        <v>13.657</v>
+      </c>
+      <c r="I21" s="34">
+        <v>0.48799999999999999</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Separate tables for adding into the paper
</commit_message>
<xml_diff>
--- a/input/core_algorithms_2022/Experiment_results.xlsx
+++ b/input/core_algorithms_2022/Experiment_results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_Devel\Repos\repos-2020-06\model-interplay-monitoring-code\input\core_algorithms_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7255EA62-772D-4652-B28B-89B41267F2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB32081-F3C0-4D82-989E-81E1656221F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33930" yWindow="-16395" windowWidth="29040" windowHeight="15990" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
   </bookViews>
   <sheets>
     <sheet name="modelSize" sheetId="6" r:id="rId1"/>
     <sheet name="conditions" sheetId="7" r:id="rId2"/>
     <sheet name="syncPoints" sheetId="8" r:id="rId3"/>
     <sheet name="modelCount" sheetId="9" r:id="rId4"/>
+    <sheet name="copy_for_AIM" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="105">
   <si>
     <t>States</t>
   </si>
@@ -314,6 +315,48 @@
   <si>
     <t>Test
 no.</t>
+  </si>
+  <si>
+    <t>GFA
+States</t>
+  </si>
+  <si>
+    <t>GFA
+Time (s)</t>
+  </si>
+  <si>
+    <t>Only Control Flow</t>
+  </si>
+  <si>
+    <t>Event
+Avg. (ms)</t>
+  </si>
+  <si>
+    <t>01 Model size without data &amp; 02 Model size with data</t>
+  </si>
+  <si>
+    <t>Control Flow &amp; Data</t>
+  </si>
+  <si>
+    <t>03 Guard placement in control flow &amp; 04 Number of guards (beginning -&gt; end)</t>
+  </si>
+  <si>
+    <t>Guard Position</t>
+  </si>
+  <si>
+    <t>Number of Guards</t>
+  </si>
+  <si>
+    <t>06 Syncronisation activity placement in control flow &amp; 07 Number of syncronisation activities (beginning -&gt; end)</t>
+  </si>
+  <si>
+    <t>Syncronisation Position</t>
+  </si>
+  <si>
+    <t>Number of Syncronisations</t>
+  </si>
+  <si>
+    <t>09 Number of input models without data &amp; 10 Number of input models with data</t>
   </si>
 </sst>
 </file>
@@ -466,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -556,6 +599,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -565,19 +614,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -896,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D70222-B554-4BB9-8CB5-22FD4E14CBB3}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -921,33 +985,33 @@
       <c r="A4" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="42" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="40"/>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="35" t="s">
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="36"/>
-      <c r="J4" s="37"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="42"/>
+      <c r="D5" s="44"/>
       <c r="E5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1200,30 +1264,30 @@
       <c r="A15" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="35" t="s">
+      <c r="C15" s="39"/>
+      <c r="D15" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="41" t="s">
+      <c r="E15" s="39"/>
+      <c r="F15" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="36"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="35" t="s">
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="K15" s="36"/>
-      <c r="L15" s="37"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="39"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="6" t="s">
         <v>12</v>
       </c>
@@ -1236,7 +1300,7 @@
       <c r="E16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="42"/>
+      <c r="F16" s="44"/>
       <c r="G16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1549,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936F52FE-6592-4EC8-BB4C-3889BAF1D620}">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:Y1048576"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6:W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1580,50 +1644,50 @@
       <c r="A4" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="35" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="41" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="36"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="35" t="s">
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="37"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="39"/>
       <c r="O4" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="P4" s="35" t="s">
+      <c r="P4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="35" t="s">
+      <c r="Q4" s="39"/>
+      <c r="R4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="36"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="35" t="s">
+      <c r="S4" s="38"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="V4" s="36"/>
-      <c r="W4" s="37"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="39"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1636,8 +1700,8 @@
       <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1656,7 +1720,7 @@
       <c r="M5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="38"/>
+      <c r="O5" s="41"/>
       <c r="P5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2204,23 +2268,23 @@
       <c r="O16" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="P16" s="35" t="s">
+      <c r="P16" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="35" t="s">
+      <c r="Q16" s="39"/>
+      <c r="R16" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="S16" s="36"/>
-      <c r="T16" s="37"/>
-      <c r="U16" s="35" t="s">
+      <c r="S16" s="38"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="V16" s="36"/>
-      <c r="W16" s="37"/>
+      <c r="V16" s="38"/>
+      <c r="W16" s="39"/>
     </row>
     <row r="17" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O17" s="38"/>
+      <c r="O17" s="41"/>
       <c r="P17" s="7" t="s">
         <v>12</v>
       </c>
@@ -2465,6 +2529,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="P16:Q16"/>
@@ -2473,13 +2544,6 @@
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="U16:W16"/>
     <mergeCell ref="O16:O17"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2495,8 +2559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7664E89F-51BA-4878-9967-5F93A0459797}">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:W1048576"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6:V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2525,49 +2589,49 @@
       <c r="A4" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="35" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="41" t="s">
+      <c r="E4" s="39"/>
+      <c r="F4" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="36"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="35" t="s">
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="37"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="39"/>
       <c r="O4" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="P4" s="41" t="s">
+      <c r="P4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="35" t="s">
+      <c r="Q4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="36"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="35" t="s">
+      <c r="R4" s="38"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="U4" s="36"/>
-      <c r="V4" s="37"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="39"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2580,8 +2644,8 @@
       <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="7" t="s">
         <v>6</v>
       </c>
@@ -2600,8 +2664,8 @@
       <c r="M5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="38"/>
-      <c r="P5" s="42"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="44"/>
       <c r="Q5" s="7" t="s">
         <v>6</v>
       </c>
@@ -3057,23 +3121,23 @@
       <c r="O15" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="P15" s="41" t="s">
+      <c r="P15" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="Q15" s="35" t="s">
+      <c r="Q15" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="R15" s="36"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="35" t="s">
+      <c r="R15" s="38"/>
+      <c r="S15" s="39"/>
+      <c r="T15" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="U15" s="36"/>
-      <c r="V15" s="37"/>
+      <c r="U15" s="38"/>
+      <c r="V15" s="39"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O16" s="38"/>
-      <c r="P16" s="42"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="44"/>
       <c r="Q16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3292,7 +3356,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="I16" sqref="I16:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3315,23 +3379,23 @@
       <c r="A4" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="42" t="s">
         <v>85</v>
       </c>
       <c r="C4" s="40"/>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="35" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="29" t="s">
         <v>86</v>
       </c>
@@ -3541,23 +3605,23 @@
       <c r="A14" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="42" t="s">
         <v>85</v>
       </c>
       <c r="C14" s="40"/>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="35" t="s">
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="29" t="s">
         <v>86</v>
       </c>
@@ -3771,4 +3835,846 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2516881A-C382-4C86-97A9-97EC547DE0A2}">
+  <dimension ref="A1:G51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:G51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="46"/>
+      <c r="B4" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+    </row>
+    <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
+        <v>0</v>
+      </c>
+      <c r="B6" s="35">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C6" s="23">
+        <v>54</v>
+      </c>
+      <c r="D6" s="36">
+        <v>0.255</v>
+      </c>
+      <c r="E6" s="35">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F6" s="23">
+        <v>80</v>
+      </c>
+      <c r="G6" s="35">
+        <v>0.28699999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="22">
+        <v>1</v>
+      </c>
+      <c r="B7" s="35">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="C7" s="23">
+        <v>272</v>
+      </c>
+      <c r="D7" s="36">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="E7" s="35">
+        <v>0.16</v>
+      </c>
+      <c r="F7" s="23">
+        <v>462</v>
+      </c>
+      <c r="G7" s="35">
+        <v>0.30399999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="22">
+        <v>2</v>
+      </c>
+      <c r="B8" s="35">
+        <v>0.152</v>
+      </c>
+      <c r="C8" s="23">
+        <v>1026</v>
+      </c>
+      <c r="D8" s="36">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="E8" s="35">
+        <v>0.83</v>
+      </c>
+      <c r="F8" s="23">
+        <v>1824</v>
+      </c>
+      <c r="G8" s="35">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="22">
+        <v>3</v>
+      </c>
+      <c r="B9" s="35">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="C9" s="23">
+        <v>3484</v>
+      </c>
+      <c r="D9" s="36">
+        <v>0.31</v>
+      </c>
+      <c r="E9" s="35">
+        <v>2.9239999999999999</v>
+      </c>
+      <c r="F9" s="23">
+        <v>6306</v>
+      </c>
+      <c r="G9" s="35">
+        <v>0.35299999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="22">
+        <v>4</v>
+      </c>
+      <c r="B10" s="35">
+        <v>2.3519999999999999</v>
+      </c>
+      <c r="C10" s="23">
+        <v>11278</v>
+      </c>
+      <c r="D10" s="36">
+        <v>0.307</v>
+      </c>
+      <c r="E10" s="35">
+        <v>10.118</v>
+      </c>
+      <c r="F10" s="23">
+        <v>20588</v>
+      </c>
+      <c r="G10" s="35">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="22">
+        <v>5</v>
+      </c>
+      <c r="B11" s="35">
+        <v>7.577</v>
+      </c>
+      <c r="C11" s="23">
+        <v>35560</v>
+      </c>
+      <c r="D11" s="36">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="E11" s="35">
+        <v>43.649000000000001</v>
+      </c>
+      <c r="F11" s="23">
+        <v>65230</v>
+      </c>
+      <c r="G11" s="35">
+        <v>0.32600000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="22">
+        <v>6</v>
+      </c>
+      <c r="B12" s="35">
+        <v>29.707999999999998</v>
+      </c>
+      <c r="C12" s="23">
+        <v>110298</v>
+      </c>
+      <c r="D12" s="36">
+        <v>0.251</v>
+      </c>
+      <c r="E12" s="35">
+        <v>209.23500000000001</v>
+      </c>
+      <c r="F12" s="23">
+        <v>202952</v>
+      </c>
+      <c r="G12" s="35">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="46"/>
+      <c r="B17" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+    </row>
+    <row r="18" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
+        <v>0</v>
+      </c>
+      <c r="B19" s="35">
+        <v>28.274000000000001</v>
+      </c>
+      <c r="C19" s="35">
+        <v>110298</v>
+      </c>
+      <c r="D19" s="36">
+        <v>0.246</v>
+      </c>
+      <c r="E19" s="35">
+        <v>28.257999999999999</v>
+      </c>
+      <c r="F19" s="35">
+        <v>110298</v>
+      </c>
+      <c r="G19" s="35">
+        <v>0.26500000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="22">
+        <v>1</v>
+      </c>
+      <c r="B20" s="35">
+        <v>36.281999999999996</v>
+      </c>
+      <c r="C20" s="23">
+        <v>112592</v>
+      </c>
+      <c r="D20" s="36">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="E20" s="35">
+        <v>35.768999999999998</v>
+      </c>
+      <c r="F20" s="23">
+        <v>112592</v>
+      </c>
+      <c r="G20" s="35">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="22">
+        <v>2</v>
+      </c>
+      <c r="B21" s="35">
+        <v>36.756</v>
+      </c>
+      <c r="C21" s="23">
+        <v>113816</v>
+      </c>
+      <c r="D21" s="36">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="E21" s="35">
+        <v>47.673000000000002</v>
+      </c>
+      <c r="F21" s="23">
+        <v>116118</v>
+      </c>
+      <c r="G21" s="35">
+        <v>0.28100000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="22">
+        <v>3</v>
+      </c>
+      <c r="B22" s="35">
+        <v>36.908000000000001</v>
+      </c>
+      <c r="C22" s="23">
+        <v>115572</v>
+      </c>
+      <c r="D22" s="36">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="E22" s="35">
+        <v>56.835000000000001</v>
+      </c>
+      <c r="F22" s="23">
+        <v>121436</v>
+      </c>
+      <c r="G22" s="35">
+        <v>0.29799999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="22">
+        <v>4</v>
+      </c>
+      <c r="B23" s="35">
+        <v>40.856000000000002</v>
+      </c>
+      <c r="C23" s="23">
+        <v>118292</v>
+      </c>
+      <c r="D23" s="36">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="E23" s="35">
+        <v>73.058000000000007</v>
+      </c>
+      <c r="F23" s="23">
+        <v>129590</v>
+      </c>
+      <c r="G23" s="35">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="22">
+        <v>5</v>
+      </c>
+      <c r="B24" s="35">
+        <v>38.173000000000002</v>
+      </c>
+      <c r="C24" s="23">
+        <v>122652</v>
+      </c>
+      <c r="D24" s="36">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="E24" s="35">
+        <v>98.23</v>
+      </c>
+      <c r="F24" s="23">
+        <v>142476</v>
+      </c>
+      <c r="G24" s="35">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="22">
+        <v>6</v>
+      </c>
+      <c r="B25" s="35">
+        <v>41.685000000000002</v>
+      </c>
+      <c r="C25" s="23">
+        <v>130076</v>
+      </c>
+      <c r="D25" s="36">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="E25" s="35">
+        <v>136.50299999999999</v>
+      </c>
+      <c r="F25" s="23">
+        <v>163958</v>
+      </c>
+      <c r="G25" s="35">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="22">
+        <v>7</v>
+      </c>
+      <c r="B26" s="35">
+        <v>47.811</v>
+      </c>
+      <c r="C26" s="23">
+        <v>143952</v>
+      </c>
+      <c r="D26" s="36">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="E26" s="35">
+        <v>212.702</v>
+      </c>
+      <c r="F26" s="35">
+        <v>202952</v>
+      </c>
+      <c r="G26" s="35">
+        <v>0.39300000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="46"/>
+      <c r="B31" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="38"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+    </row>
+    <row r="32" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
+        <v>0</v>
+      </c>
+      <c r="B33" s="35">
+        <v>27.649000000000001</v>
+      </c>
+      <c r="C33" s="35">
+        <v>110298</v>
+      </c>
+      <c r="D33" s="36">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="E33" s="35">
+        <v>27.878</v>
+      </c>
+      <c r="F33" s="35">
+        <v>110298</v>
+      </c>
+      <c r="G33" s="35">
+        <v>0.254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="22">
+        <v>1</v>
+      </c>
+      <c r="B34" s="35">
+        <v>28.402999999999999</v>
+      </c>
+      <c r="C34" s="23">
+        <v>107463</v>
+      </c>
+      <c r="D34" s="36">
+        <v>0.255</v>
+      </c>
+      <c r="E34" s="35">
+        <v>28.166</v>
+      </c>
+      <c r="F34" s="23">
+        <v>107463</v>
+      </c>
+      <c r="G34" s="35">
+        <v>0.25900000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="22">
+        <v>2</v>
+      </c>
+      <c r="B35" s="35">
+        <v>26.989000000000001</v>
+      </c>
+      <c r="C35" s="23">
+        <v>102891</v>
+      </c>
+      <c r="D35" s="36">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="E35" s="35">
+        <v>28.323</v>
+      </c>
+      <c r="F35" s="23">
+        <v>103228</v>
+      </c>
+      <c r="G35" s="35">
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="22">
+        <v>3</v>
+      </c>
+      <c r="B36" s="35">
+        <v>24.521999999999998</v>
+      </c>
+      <c r="C36" s="23">
+        <v>96521</v>
+      </c>
+      <c r="D36" s="36">
+        <v>0.248</v>
+      </c>
+      <c r="E36" s="35">
+        <v>27.428000000000001</v>
+      </c>
+      <c r="F36" s="23">
+        <v>97173</v>
+      </c>
+      <c r="G36" s="35">
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="22">
+        <v>4</v>
+      </c>
+      <c r="B37" s="35">
+        <v>22.553000000000001</v>
+      </c>
+      <c r="C37" s="23">
+        <v>88323</v>
+      </c>
+      <c r="D37" s="36">
+        <v>0.248</v>
+      </c>
+      <c r="E37" s="35">
+        <v>25.245000000000001</v>
+      </c>
+      <c r="F37" s="23">
+        <v>88866</v>
+      </c>
+      <c r="G37" s="35">
+        <v>0.248</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="22">
+        <v>5</v>
+      </c>
+      <c r="B38" s="35">
+        <v>20.119</v>
+      </c>
+      <c r="C38" s="23">
+        <v>80073</v>
+      </c>
+      <c r="D38" s="36">
+        <v>0.254</v>
+      </c>
+      <c r="E38" s="35">
+        <v>22.638000000000002</v>
+      </c>
+      <c r="F38" s="23">
+        <v>78631</v>
+      </c>
+      <c r="G38" s="35">
+        <v>0.27900000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="22">
+        <v>6</v>
+      </c>
+      <c r="B39" s="35">
+        <v>18.905000000000001</v>
+      </c>
+      <c r="C39" s="23">
+        <v>79949</v>
+      </c>
+      <c r="D39" s="36">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="E39" s="35">
+        <v>21.321000000000002</v>
+      </c>
+      <c r="F39" s="23">
+        <v>69870</v>
+      </c>
+      <c r="G39" s="35">
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="46"/>
+      <c r="B44" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="38"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+    </row>
+    <row r="45" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="15">
+        <v>0</v>
+      </c>
+      <c r="B46" s="35">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C46" s="23">
+        <v>4</v>
+      </c>
+      <c r="D46" s="36">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="E46" s="35">
+        <v>0.02</v>
+      </c>
+      <c r="F46" s="23">
+        <v>6</v>
+      </c>
+      <c r="G46" s="36">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="22">
+        <v>1</v>
+      </c>
+      <c r="B47" s="35">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C47" s="23">
+        <v>36</v>
+      </c>
+      <c r="D47" s="36">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="E47" s="35">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F47" s="23">
+        <v>64</v>
+      </c>
+      <c r="G47" s="36">
+        <v>0.38700000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="22">
+        <v>2</v>
+      </c>
+      <c r="B48" s="35">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="C48" s="23">
+        <v>216</v>
+      </c>
+      <c r="D48" s="36">
+        <v>0.378</v>
+      </c>
+      <c r="E48" s="35">
+        <v>0.111</v>
+      </c>
+      <c r="F48" s="23">
+        <v>512</v>
+      </c>
+      <c r="G48" s="36">
+        <v>0.45900000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="22">
+        <v>3</v>
+      </c>
+      <c r="B49" s="35">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="C49" s="23">
+        <v>1296</v>
+      </c>
+      <c r="D49" s="36">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="E49" s="35">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="F49" s="23">
+        <v>4096</v>
+      </c>
+      <c r="G49" s="36">
+        <v>0.50800000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="22">
+        <v>4</v>
+      </c>
+      <c r="B50" s="35">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="C50" s="23">
+        <v>7776</v>
+      </c>
+      <c r="D50" s="36">
+        <v>0.441</v>
+      </c>
+      <c r="E50" s="35">
+        <v>5.1369999999999996</v>
+      </c>
+      <c r="F50" s="23">
+        <v>32768</v>
+      </c>
+      <c r="G50" s="36">
+        <v>0.438</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="22">
+        <v>5</v>
+      </c>
+      <c r="B51" s="35">
+        <v>2.7010000000000001</v>
+      </c>
+      <c r="C51" s="23">
+        <v>46656</v>
+      </c>
+      <c r="D51" s="36">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="E51" s="35">
+        <v>54.033999999999999</v>
+      </c>
+      <c r="F51" s="23">
+        <v>262144</v>
+      </c>
+      <c r="G51" s="36">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes for running the scalability tests from command line
</commit_message>
<xml_diff>
--- a/input/core_algorithms_2022/Experiment_results.xlsx
+++ b/input/core_algorithms_2022/Experiment_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UT_Devel\Repos\repos-2020-06\model-interplay-monitoring-code\input\core_algorithms_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB32081-F3C0-4D82-989E-81E1656221F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E944953F-317F-4849-8E8E-27126AFAACD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8E243F24-B93C-40CA-AE61-5F4BEE95CD75}"/>
   </bookViews>
   <sheets>
     <sheet name="modelSize" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="105">
   <si>
     <t>States</t>
   </si>
@@ -509,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -605,6 +605,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -631,18 +652,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -960,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D70222-B554-4BB9-8CB5-22FD4E14CBB3}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:F12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -982,36 +991,36 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="43" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="37" t="s">
+      <c r="F4" s="45"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1261,33 +1270,33 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="37" t="s">
+      <c r="C15" s="46"/>
+      <c r="D15" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="43" t="s">
+      <c r="E15" s="46"/>
+      <c r="F15" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="37" t="s">
+      <c r="H15" s="45"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="K15" s="38"/>
-      <c r="L15" s="39"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="46"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="6" t="s">
         <v>12</v>
       </c>
@@ -1300,7 +1309,7 @@
       <c r="E16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="44"/>
+      <c r="F16" s="51"/>
       <c r="G16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1641,53 +1650,53 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="37" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="43" t="s">
+      <c r="E4" s="46"/>
+      <c r="F4" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="37" t="s">
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="38"/>
-      <c r="M4" s="39"/>
-      <c r="O4" s="40" t="s">
+      <c r="L4" s="45"/>
+      <c r="M4" s="46"/>
+      <c r="O4" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="P4" s="37" t="s">
+      <c r="P4" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="37" t="s">
+      <c r="Q4" s="46"/>
+      <c r="R4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="38"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="37" t="s">
+      <c r="S4" s="45"/>
+      <c r="T4" s="46"/>
+      <c r="U4" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="V4" s="38"/>
-      <c r="W4" s="39"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="46"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1700,8 +1709,8 @@
       <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
       <c r="H5" s="7" t="s">
         <v>6</v>
       </c>
@@ -1720,7 +1729,7 @@
       <c r="M5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="41"/>
+      <c r="O5" s="48"/>
       <c r="P5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2265,26 +2274,26 @@
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="O16" s="40" t="s">
+      <c r="O16" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="P16" s="37" t="s">
+      <c r="P16" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="37" t="s">
+      <c r="Q16" s="46"/>
+      <c r="R16" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="S16" s="38"/>
-      <c r="T16" s="39"/>
-      <c r="U16" s="37" t="s">
+      <c r="S16" s="45"/>
+      <c r="T16" s="46"/>
+      <c r="U16" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="V16" s="38"/>
-      <c r="W16" s="39"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="46"/>
     </row>
     <row r="17" spans="15:24" x14ac:dyDescent="0.3">
-      <c r="O17" s="41"/>
+      <c r="O17" s="48"/>
       <c r="P17" s="7" t="s">
         <v>12</v>
       </c>
@@ -2529,13 +2538,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:J4"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="P16:Q16"/>
@@ -2544,6 +2546,13 @@
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="U16:W16"/>
     <mergeCell ref="O16:O17"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2586,52 +2595,52 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="37" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="43" t="s">
+      <c r="E4" s="46"/>
+      <c r="F4" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="37" t="s">
+      <c r="I4" s="45"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="38"/>
-      <c r="M4" s="39"/>
-      <c r="O4" s="40" t="s">
+      <c r="L4" s="45"/>
+      <c r="M4" s="46"/>
+      <c r="O4" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="P4" s="43" t="s">
+      <c r="P4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="38"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="37" t="s">
+      <c r="R4" s="45"/>
+      <c r="S4" s="46"/>
+      <c r="T4" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="U4" s="38"/>
-      <c r="V4" s="39"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="46"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2644,8 +2653,8 @@
       <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
       <c r="H5" s="7" t="s">
         <v>6</v>
       </c>
@@ -2664,8 +2673,8 @@
       <c r="M5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="41"/>
-      <c r="P5" s="44"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="51"/>
       <c r="Q5" s="7" t="s">
         <v>6</v>
       </c>
@@ -3118,26 +3127,26 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O15" s="40" t="s">
+      <c r="O15" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="P15" s="43" t="s">
+      <c r="P15" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="Q15" s="37" t="s">
+      <c r="Q15" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="R15" s="38"/>
-      <c r="S15" s="39"/>
-      <c r="T15" s="37" t="s">
+      <c r="R15" s="45"/>
+      <c r="S15" s="46"/>
+      <c r="T15" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="U15" s="38"/>
-      <c r="V15" s="39"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="46"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O16" s="41"/>
-      <c r="P16" s="44"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="51"/>
       <c r="Q16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3376,26 +3385,26 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="37" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="37" t="s">
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="46"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="29" t="s">
         <v>86</v>
       </c>
@@ -3602,26 +3611,26 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="37" t="s">
+      <c r="C14" s="47"/>
+      <c r="D14" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="37" t="s">
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="46"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="29" t="s">
         <v>86</v>
       </c>
@@ -3839,10 +3848,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2516881A-C382-4C86-97A9-97EC547DE0A2}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:G51"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3861,38 +3870,38 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
-      <c r="B4" s="37" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
     </row>
     <row r="5" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="42" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4063,38 +4072,38 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="46"/>
-      <c r="B17" s="37" t="s">
+      <c r="A17" s="40"/>
+      <c r="B17" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="45" t="s">
+      <c r="C17" s="45"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
     </row>
     <row r="18" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="48" t="s">
+      <c r="E18" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="48" t="s">
+      <c r="F18" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="G18" s="42" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4282,397 +4291,775 @@
         <v>0.39300000000000002</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="40"/>
+      <c r="B28" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+    </row>
+    <row r="29" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>95</v>
+      </c>
+    </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>101</v>
+      <c r="A30" s="22">
+        <v>1</v>
+      </c>
+      <c r="B30" s="37">
+        <v>35.768999999999998</v>
+      </c>
+      <c r="C30" s="39">
+        <v>112592</v>
+      </c>
+      <c r="D30" s="38">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="E30" s="37">
+        <v>36.281999999999996</v>
+      </c>
+      <c r="F30" s="39">
+        <v>112592</v>
+      </c>
+      <c r="G30" s="37">
+        <v>0.30199999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="46"/>
-      <c r="B31" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-    </row>
-    <row r="32" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="E32" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="G32" s="48" t="s">
-        <v>95</v>
+      <c r="A31" s="22">
+        <v>2</v>
+      </c>
+      <c r="B31" s="37">
+        <v>47.673000000000002</v>
+      </c>
+      <c r="C31" s="39">
+        <v>116118</v>
+      </c>
+      <c r="D31" s="38">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="E31" s="37">
+        <v>36.756</v>
+      </c>
+      <c r="F31" s="39">
+        <v>113816</v>
+      </c>
+      <c r="G31" s="37">
+        <v>0.26500000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="22">
+        <v>3</v>
+      </c>
+      <c r="B32" s="37">
+        <v>56.835000000000001</v>
+      </c>
+      <c r="C32" s="39">
+        <v>121436</v>
+      </c>
+      <c r="D32" s="38">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="E32" s="37">
+        <v>36.908000000000001</v>
+      </c>
+      <c r="F32" s="39">
+        <v>115572</v>
+      </c>
+      <c r="G32" s="37">
+        <v>0.26700000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="15">
-        <v>0</v>
-      </c>
-      <c r="B33" s="35">
-        <v>27.649000000000001</v>
-      </c>
-      <c r="C33" s="35">
-        <v>110298</v>
-      </c>
-      <c r="D33" s="36">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="E33" s="35">
-        <v>27.878</v>
-      </c>
-      <c r="F33" s="35">
-        <v>110298</v>
-      </c>
-      <c r="G33" s="35">
-        <v>0.254</v>
+      <c r="A33" s="22">
+        <v>4</v>
+      </c>
+      <c r="B33" s="37">
+        <v>73.058000000000007</v>
+      </c>
+      <c r="C33" s="39">
+        <v>129590</v>
+      </c>
+      <c r="D33" s="38">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="E33" s="37">
+        <v>40.856000000000002</v>
+      </c>
+      <c r="F33" s="39">
+        <v>118292</v>
+      </c>
+      <c r="G33" s="37">
+        <v>0.28199999999999997</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="22">
-        <v>1</v>
-      </c>
-      <c r="B34" s="35">
-        <v>28.402999999999999</v>
-      </c>
-      <c r="C34" s="23">
-        <v>107463</v>
-      </c>
-      <c r="D34" s="36">
-        <v>0.255</v>
-      </c>
-      <c r="E34" s="35">
-        <v>28.166</v>
-      </c>
-      <c r="F34" s="23">
-        <v>107463</v>
-      </c>
-      <c r="G34" s="35">
-        <v>0.25900000000000001</v>
+        <v>5</v>
+      </c>
+      <c r="B34" s="37">
+        <v>98.23</v>
+      </c>
+      <c r="C34" s="39">
+        <v>142476</v>
+      </c>
+      <c r="D34" s="38">
+        <v>0.32</v>
+      </c>
+      <c r="E34" s="37">
+        <v>38.173000000000002</v>
+      </c>
+      <c r="F34" s="39">
+        <v>122652</v>
+      </c>
+      <c r="G34" s="37">
+        <v>0.26500000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
-        <v>2</v>
-      </c>
-      <c r="B35" s="35">
-        <v>26.989000000000001</v>
-      </c>
-      <c r="C35" s="23">
-        <v>102891</v>
-      </c>
-      <c r="D35" s="36">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="E35" s="35">
-        <v>28.323</v>
-      </c>
-      <c r="F35" s="23">
-        <v>103228</v>
-      </c>
-      <c r="G35" s="35">
-        <v>0.249</v>
+        <v>6</v>
+      </c>
+      <c r="B35" s="37">
+        <v>136.50299999999999</v>
+      </c>
+      <c r="C35" s="39">
+        <v>163958</v>
+      </c>
+      <c r="D35" s="38">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="E35" s="37">
+        <v>41.685000000000002</v>
+      </c>
+      <c r="F35" s="39">
+        <v>130076</v>
+      </c>
+      <c r="G35" s="37">
+        <v>0.26900000000000002</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="22">
+        <v>7</v>
+      </c>
+      <c r="B36" s="37">
+        <v>212.702</v>
+      </c>
+      <c r="C36" s="37">
+        <v>202952</v>
+      </c>
+      <c r="D36" s="38">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="E36" s="37">
+        <v>47.811</v>
+      </c>
+      <c r="F36" s="39">
+        <v>143952</v>
+      </c>
+      <c r="G36" s="37">
+        <v>0.26900000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="40"/>
+      <c r="B40" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="45"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+    </row>
+    <row r="41" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="15">
+        <v>0</v>
+      </c>
+      <c r="B42" s="35">
+        <v>27.649000000000001</v>
+      </c>
+      <c r="C42" s="35">
+        <v>110298</v>
+      </c>
+      <c r="D42" s="36">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="E42" s="35">
+        <v>27.878</v>
+      </c>
+      <c r="F42" s="35">
+        <v>110298</v>
+      </c>
+      <c r="G42" s="35">
+        <v>0.254</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="22">
+        <v>1</v>
+      </c>
+      <c r="B43" s="35">
+        <v>28.402999999999999</v>
+      </c>
+      <c r="C43" s="23">
+        <v>107463</v>
+      </c>
+      <c r="D43" s="36">
+        <v>0.255</v>
+      </c>
+      <c r="E43" s="35">
+        <v>28.166</v>
+      </c>
+      <c r="F43" s="23">
+        <v>107463</v>
+      </c>
+      <c r="G43" s="35">
+        <v>0.25900000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="22">
+        <v>2</v>
+      </c>
+      <c r="B44" s="35">
+        <v>26.989000000000001</v>
+      </c>
+      <c r="C44" s="23">
+        <v>102891</v>
+      </c>
+      <c r="D44" s="36">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="E44" s="35">
+        <v>28.323</v>
+      </c>
+      <c r="F44" s="23">
+        <v>103228</v>
+      </c>
+      <c r="G44" s="35">
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="22">
         <v>3</v>
       </c>
-      <c r="B36" s="35">
+      <c r="B45" s="35">
         <v>24.521999999999998</v>
       </c>
-      <c r="C36" s="23">
+      <c r="C45" s="23">
         <v>96521</v>
       </c>
-      <c r="D36" s="36">
+      <c r="D45" s="36">
         <v>0.248</v>
       </c>
-      <c r="E36" s="35">
+      <c r="E45" s="35">
         <v>27.428000000000001</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F45" s="23">
         <v>97173</v>
       </c>
-      <c r="G36" s="35">
+      <c r="G45" s="35">
         <v>0.25600000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="22">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="22">
         <v>4</v>
       </c>
-      <c r="B37" s="35">
+      <c r="B46" s="35">
         <v>22.553000000000001</v>
       </c>
-      <c r="C37" s="23">
+      <c r="C46" s="23">
         <v>88323</v>
       </c>
-      <c r="D37" s="36">
+      <c r="D46" s="36">
         <v>0.248</v>
       </c>
-      <c r="E37" s="35">
+      <c r="E46" s="35">
         <v>25.245000000000001</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F46" s="23">
         <v>88866</v>
       </c>
-      <c r="G37" s="35">
+      <c r="G46" s="35">
         <v>0.248</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="22">
-        <v>5</v>
-      </c>
-      <c r="B38" s="35">
-        <v>20.119</v>
-      </c>
-      <c r="C38" s="23">
-        <v>80073</v>
-      </c>
-      <c r="D38" s="36">
-        <v>0.254</v>
-      </c>
-      <c r="E38" s="35">
-        <v>22.638000000000002</v>
-      </c>
-      <c r="F38" s="23">
-        <v>78631</v>
-      </c>
-      <c r="G38" s="35">
-        <v>0.27900000000000003</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="22">
-        <v>6</v>
-      </c>
-      <c r="B39" s="35">
-        <v>18.905000000000001</v>
-      </c>
-      <c r="C39" s="23">
-        <v>79949</v>
-      </c>
-      <c r="D39" s="36">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="E39" s="35">
-        <v>21.321000000000002</v>
-      </c>
-      <c r="F39" s="23">
-        <v>69870</v>
-      </c>
-      <c r="G39" s="35">
-        <v>0.249</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="46"/>
-      <c r="B44" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="38"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-    </row>
-    <row r="45" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="E45" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="F45" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="G45" s="48" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="15">
-        <v>0</v>
-      </c>
-      <c r="B46" s="35">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="C46" s="23">
-        <v>4</v>
-      </c>
-      <c r="D46" s="36">
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="E46" s="35">
-        <v>0.02</v>
-      </c>
-      <c r="F46" s="23">
-        <v>6</v>
-      </c>
-      <c r="G46" s="36">
-        <v>0.311</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B47" s="35">
-        <v>2.3E-2</v>
+        <v>20.119</v>
       </c>
       <c r="C47" s="23">
-        <v>36</v>
+        <v>80073</v>
       </c>
       <c r="D47" s="36">
-        <v>0.34200000000000003</v>
+        <v>0.254</v>
       </c>
       <c r="E47" s="35">
-        <v>4.1000000000000002E-2</v>
+        <v>22.638000000000002</v>
       </c>
       <c r="F47" s="23">
-        <v>64</v>
-      </c>
-      <c r="G47" s="36">
-        <v>0.38700000000000001</v>
+        <v>78631</v>
+      </c>
+      <c r="G47" s="35">
+        <v>0.27900000000000003</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="22">
+        <v>6</v>
+      </c>
+      <c r="B48" s="35">
+        <v>18.905000000000001</v>
+      </c>
+      <c r="C48" s="23">
+        <v>79949</v>
+      </c>
+      <c r="D48" s="36">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="E48" s="35">
+        <v>21.321000000000002</v>
+      </c>
+      <c r="F48" s="23">
+        <v>69870</v>
+      </c>
+      <c r="G48" s="35">
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="40"/>
+      <c r="B50" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="52"/>
+      <c r="D50" s="52"/>
+      <c r="E50" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+    </row>
+    <row r="51" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51" s="42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="22">
+        <v>1</v>
+      </c>
+      <c r="B52" s="37">
+        <v>28.166</v>
+      </c>
+      <c r="C52" s="39">
+        <v>107463</v>
+      </c>
+      <c r="D52" s="38">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="E52" s="37">
+        <v>28.402999999999999</v>
+      </c>
+      <c r="F52" s="39">
+        <v>107463</v>
+      </c>
+      <c r="G52" s="37">
+        <v>0.255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="22">
         <v>2</v>
       </c>
-      <c r="B48" s="35">
+      <c r="B53" s="37">
+        <v>28.323</v>
+      </c>
+      <c r="C53" s="39">
+        <v>103228</v>
+      </c>
+      <c r="D53" s="38">
+        <v>0.249</v>
+      </c>
+      <c r="E53" s="37">
+        <v>26.989000000000001</v>
+      </c>
+      <c r="F53" s="39">
+        <v>102891</v>
+      </c>
+      <c r="G53" s="37">
+        <v>0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="22">
+        <v>3</v>
+      </c>
+      <c r="B54" s="37">
+        <v>27.428000000000001</v>
+      </c>
+      <c r="C54" s="39">
+        <v>97173</v>
+      </c>
+      <c r="D54" s="38">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="E54" s="37">
+        <v>24.521999999999998</v>
+      </c>
+      <c r="F54" s="39">
+        <v>96521</v>
+      </c>
+      <c r="G54" s="37">
+        <v>0.248</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="22">
+        <v>4</v>
+      </c>
+      <c r="B55" s="37">
+        <v>25.245000000000001</v>
+      </c>
+      <c r="C55" s="39">
+        <v>88866</v>
+      </c>
+      <c r="D55" s="38">
+        <v>0.248</v>
+      </c>
+      <c r="E55" s="37">
+        <v>22.553000000000001</v>
+      </c>
+      <c r="F55" s="39">
+        <v>88323</v>
+      </c>
+      <c r="G55" s="37">
+        <v>0.248</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="22">
+        <v>5</v>
+      </c>
+      <c r="B56" s="37">
+        <v>22.638000000000002</v>
+      </c>
+      <c r="C56" s="39">
+        <v>78631</v>
+      </c>
+      <c r="D56" s="38">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="E56" s="37">
+        <v>20.119</v>
+      </c>
+      <c r="F56" s="39">
+        <v>80073</v>
+      </c>
+      <c r="G56" s="37">
+        <v>0.254</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="22">
+        <v>6</v>
+      </c>
+      <c r="B57" s="37">
+        <v>21.321000000000002</v>
+      </c>
+      <c r="C57" s="39">
+        <v>69870</v>
+      </c>
+      <c r="D57" s="38">
+        <v>0.249</v>
+      </c>
+      <c r="E57" s="37">
+        <v>18.905000000000001</v>
+      </c>
+      <c r="F57" s="39">
+        <v>79949</v>
+      </c>
+      <c r="G57" s="37">
+        <v>0.24299999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="40"/>
+      <c r="B61" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="45"/>
+      <c r="D61" s="46"/>
+      <c r="E61" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="F61" s="52"/>
+      <c r="G61" s="52"/>
+    </row>
+    <row r="62" spans="1:7" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A62" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C62" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E62" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F62" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G62" s="42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="15">
+        <v>0</v>
+      </c>
+      <c r="B63" s="35">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C63" s="23">
+        <v>4</v>
+      </c>
+      <c r="D63" s="36">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="E63" s="35">
+        <v>0.02</v>
+      </c>
+      <c r="F63" s="23">
+        <v>6</v>
+      </c>
+      <c r="G63" s="36">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="22">
+        <v>1</v>
+      </c>
+      <c r="B64" s="35">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C64" s="23">
+        <v>36</v>
+      </c>
+      <c r="D64" s="36">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="E64" s="35">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F64" s="23">
+        <v>64</v>
+      </c>
+      <c r="G64" s="36">
+        <v>0.38700000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="22">
+        <v>2</v>
+      </c>
+      <c r="B65" s="35">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="C48" s="23">
+      <c r="C65" s="23">
         <v>216</v>
       </c>
-      <c r="D48" s="36">
+      <c r="D65" s="36">
         <v>0.378</v>
       </c>
-      <c r="E48" s="35">
+      <c r="E65" s="35">
         <v>0.111</v>
       </c>
-      <c r="F48" s="23">
+      <c r="F65" s="23">
         <v>512</v>
       </c>
-      <c r="G48" s="36">
+      <c r="G65" s="36">
         <v>0.45900000000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="22">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="22">
         <v>3</v>
       </c>
-      <c r="B49" s="35">
+      <c r="B66" s="35">
         <v>0.11600000000000001</v>
       </c>
-      <c r="C49" s="23">
+      <c r="C66" s="23">
         <v>1296</v>
       </c>
-      <c r="D49" s="36">
+      <c r="D66" s="36">
         <v>0.41499999999999998</v>
       </c>
-      <c r="E49" s="35">
+      <c r="E66" s="35">
         <v>0.75600000000000001</v>
       </c>
-      <c r="F49" s="23">
+      <c r="F66" s="23">
         <v>4096</v>
       </c>
-      <c r="G49" s="36">
+      <c r="G66" s="36">
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="22">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="22">
         <v>4</v>
       </c>
-      <c r="B50" s="35">
+      <c r="B67" s="35">
         <v>0.42899999999999999</v>
       </c>
-      <c r="C50" s="23">
+      <c r="C67" s="23">
         <v>7776</v>
       </c>
-      <c r="D50" s="36">
+      <c r="D67" s="36">
         <v>0.441</v>
       </c>
-      <c r="E50" s="35">
+      <c r="E67" s="35">
         <v>5.1369999999999996</v>
       </c>
-      <c r="F50" s="23">
+      <c r="F67" s="23">
         <v>32768</v>
       </c>
-      <c r="G50" s="36">
+      <c r="G67" s="36">
         <v>0.438</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="22">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="22">
         <v>5</v>
       </c>
-      <c r="B51" s="35">
+      <c r="B68" s="35">
         <v>2.7010000000000001</v>
       </c>
-      <c r="C51" s="23">
+      <c r="C68" s="23">
         <v>46656</v>
       </c>
-      <c r="D51" s="36">
+      <c r="D68" s="36">
         <v>0.48799999999999999</v>
       </c>
-      <c r="E51" s="35">
+      <c r="E68" s="35">
         <v>54.033999999999999</v>
       </c>
-      <c r="F51" s="23">
+      <c r="F68" s="23">
         <v>262144</v>
       </c>
-      <c r="G51" s="36">
+      <c r="G68" s="36">
         <v>0.48799999999999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
+  <mergeCells count="12">
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="E61:G61"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B50:D50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>